<commit_message>
Update with new data from Brownie
</commit_message>
<xml_diff>
--- a/figures+tables/Compare_OpenET-WIMAS_LEMA_allts_FitStats_Formatted.xlsx
+++ b/figures+tables/Compare_OpenET-WIMAS_LEMA_allts_FitStats_Formatted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s947z036\WorkGits\SD-6_MapWaterConservation\figures+tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD088A53-290F-494D-824A-3E10E839A5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCF9605-2439-4633-98C4-DC9720E9E804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="780" windowWidth="16575" windowHeight="16335" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="copy raw data here" sheetId="1" r:id="rId1"/>
@@ -442,9 +442,6 @@
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -466,21 +463,21 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -490,6 +487,9 @@
     <xf numFmtId="9" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -774,7 +774,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="A1:XFD1048576"/>
+      <selection activeCell="D21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,40 +825,40 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>11.2</v>
+        <v>4.2</v>
       </c>
       <c r="C2">
-        <v>-5.3</v>
+        <v>-11.2</v>
       </c>
       <c r="D2">
-        <v>53</v>
+        <v>43.3</v>
       </c>
       <c r="E2">
-        <v>1.0521325881157999</v>
+        <v>1.01421166801854</v>
       </c>
       <c r="F2">
-        <v>1.05135495334442</v>
+        <v>1.0566785240185399</v>
       </c>
       <c r="G2">
-        <v>1.12663722334442</v>
+        <v>1.13210450601854</v>
       </c>
       <c r="H2">
-        <v>0.86376164822378598</v>
+        <v>0.863922892747502</v>
       </c>
       <c r="I2">
-        <v>0.80618789921720402</v>
+        <v>0.80795694980699195</v>
       </c>
       <c r="J2">
-        <v>0.65203593676152205</v>
+        <v>0.65750235090564702</v>
       </c>
       <c r="K2">
-        <v>3.3374783120993698</v>
+        <v>3.1335955590101099</v>
       </c>
       <c r="L2">
-        <v>3.0269811296883899</v>
+        <v>2.8449553227162201</v>
       </c>
       <c r="M2">
-        <v>3.0712426252462901</v>
+        <v>2.8956860816209802</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -866,40 +866,40 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>54.7</v>
+        <v>44.9</v>
       </c>
       <c r="C3">
-        <v>45.4</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="D3">
-        <v>96.5</v>
+        <v>84.1</v>
       </c>
       <c r="E3">
-        <v>1.3316947738145499</v>
+        <v>1.27413992293317</v>
       </c>
       <c r="F3">
-        <v>1.2724853541158001</v>
+        <v>1.22370623293317</v>
       </c>
       <c r="G3">
-        <v>1.83591235817483</v>
+        <v>1.7079850700619399</v>
       </c>
       <c r="H3">
-        <v>0.96907780717402503</v>
+        <v>0.96403640732375395</v>
       </c>
       <c r="I3">
-        <v>0.90676330233740599</v>
+        <v>0.90247532090521798</v>
       </c>
       <c r="J3">
-        <v>0.83250710429626895</v>
+        <v>0.83748434156848695</v>
       </c>
       <c r="K3">
-        <v>4.3378172557114398</v>
+        <v>4.0619192469853198</v>
       </c>
       <c r="L3">
-        <v>3.96624857761035</v>
+        <v>3.7149885047470099</v>
       </c>
       <c r="M3">
-        <v>3.96295203219139</v>
+        <v>3.73206031795227</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -907,40 +907,40 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>21.6</v>
+        <v>13.9</v>
       </c>
       <c r="C4">
-        <v>14.1</v>
+        <v>6.9</v>
       </c>
       <c r="D4">
-        <v>63.2</v>
+        <v>53</v>
       </c>
       <c r="E4">
-        <v>1.2001283241158001</v>
+        <v>1.1513136169331699</v>
       </c>
       <c r="F4">
-        <v>1.0342946601158001</v>
+        <v>0.98552670093317096</v>
       </c>
       <c r="G4">
-        <v>1.3103127278145501</v>
+        <v>1.2129977769331699</v>
       </c>
       <c r="H4">
-        <v>0.96549445281805502</v>
+        <v>0.960542507354751</v>
       </c>
       <c r="I4">
-        <v>0.923217263031333</v>
+        <v>0.92077137459599301</v>
       </c>
       <c r="J4">
-        <v>0.854431416194254</v>
+        <v>0.85730046747484201</v>
       </c>
       <c r="K4">
-        <v>3.9460191028290601</v>
+        <v>3.6951717519075999</v>
       </c>
       <c r="L4">
-        <v>3.5622311854927702</v>
+        <v>3.3400324767145899</v>
       </c>
       <c r="M4">
-        <v>3.7016718989408801</v>
+        <v>3.4815001151263001</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -948,40 +948,40 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>-11.1</v>
+        <v>-16.7</v>
       </c>
       <c r="C5">
-        <v>-18.5</v>
+        <v>-23.7</v>
       </c>
       <c r="D5">
-        <v>21.8</v>
+        <v>14.1</v>
       </c>
       <c r="E5">
-        <v>1.1044924468520101</v>
+        <v>1.1634389124664599</v>
       </c>
       <c r="F5">
-        <v>1.1389014208520101</v>
+        <v>1.1978005744664599</v>
       </c>
       <c r="G5">
-        <v>1.23074981734442</v>
+        <v>1.23618700001854</v>
       </c>
       <c r="H5">
-        <v>0.894122469439247</v>
+        <v>0.88848660049837003</v>
       </c>
       <c r="I5">
-        <v>0.83477331068213401</v>
+        <v>0.83297081032059195</v>
       </c>
       <c r="J5">
-        <v>0.82944973105878195</v>
+        <v>0.83107424273178199</v>
       </c>
       <c r="K5">
-        <v>3.57444354830821</v>
+        <v>3.34524192817543</v>
       </c>
       <c r="L5">
-        <v>3.2202795644670599</v>
+        <v>3.0201145318680198</v>
       </c>
       <c r="M5">
-        <v>3.91229008459465</v>
+        <v>3.6767724909794302</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -989,40 +989,40 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>10.4</v>
+        <v>3.4</v>
       </c>
       <c r="C6">
-        <v>1.5</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="D6">
-        <v>51.6</v>
+        <v>42.1</v>
       </c>
       <c r="E6">
-        <v>1.1031031576234001</v>
+        <v>1.1078974873810801</v>
       </c>
       <c r="F6">
-        <v>0.913943772852019</v>
+        <v>0.97308437046646201</v>
       </c>
       <c r="G6">
-        <v>1.1440476861158</v>
+        <v>1.09541417093317</v>
       </c>
       <c r="H6">
-        <v>0.95321227213915605</v>
+        <v>0.948445807703301</v>
       </c>
       <c r="I6">
-        <v>0.90836205052499497</v>
+        <v>0.90651028712940196</v>
       </c>
       <c r="J6">
-        <v>0.82137053726634002</v>
+        <v>0.82402691999106004</v>
       </c>
       <c r="K6">
-        <v>3.85586323818004</v>
+        <v>3.6110324960609801</v>
       </c>
       <c r="L6">
-        <v>3.47859052554952</v>
+        <v>3.2626810758104599</v>
       </c>
       <c r="M6">
-        <v>3.67247715845583</v>
+        <v>3.4540316842252601</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1030,40 +1030,40 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>112.9</v>
+        <v>99.5</v>
       </c>
       <c r="C7">
-        <v>92.7</v>
+        <v>80.599999999999994</v>
       </c>
       <c r="D7">
-        <v>158.6</v>
+        <v>142.30000000000001</v>
       </c>
       <c r="E7">
-        <v>2.14756867017483</v>
+        <v>2.01920330806194</v>
       </c>
       <c r="F7">
-        <v>1.76381402217483</v>
+        <v>1.6356503500619399</v>
       </c>
       <c r="G7">
-        <v>3.01753937417483</v>
+        <v>2.88885652806194</v>
       </c>
       <c r="H7">
-        <v>0.98516090863149497</v>
+        <v>0.98109238708060997</v>
       </c>
       <c r="I7">
-        <v>0.94341262423966099</v>
+        <v>0.940742373788099</v>
       </c>
       <c r="J7">
-        <v>0.79954221208533605</v>
+        <v>0.79998727147353899</v>
       </c>
       <c r="K7">
-        <v>3.6617285652198799</v>
+        <v>3.4311334422637598</v>
       </c>
       <c r="L7">
-        <v>3.25056417293065</v>
+        <v>3.0480392336422102</v>
       </c>
       <c r="M7">
-        <v>3.04284663926475</v>
+        <v>2.8587905302868402</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1071,40 +1071,40 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>-0.9</v>
+        <v>-7.1</v>
       </c>
       <c r="C8">
-        <v>7.7</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>36.4</v>
+        <v>27.8</v>
       </c>
       <c r="E8">
-        <v>1.1344329836233999</v>
+        <v>1.13914671338108</v>
       </c>
       <c r="F8">
-        <v>0.94102003762340003</v>
+        <v>0.94583763538108701</v>
       </c>
       <c r="G8">
-        <v>1.0968711601158001</v>
+        <v>1.04815943493317</v>
       </c>
       <c r="H8">
-        <v>0.94416586775407096</v>
+        <v>0.93563642400835201</v>
       </c>
       <c r="I8">
-        <v>0.91687333267720295</v>
+        <v>0.91094405569218395</v>
       </c>
       <c r="J8">
-        <v>0.89648646126581599</v>
+        <v>0.89904925620429799</v>
       </c>
       <c r="K8">
-        <v>3.5464378974631199</v>
+        <v>3.3143642744465498</v>
       </c>
       <c r="L8">
-        <v>3.4014070995100498</v>
+        <v>3.1830707103834901</v>
       </c>
       <c r="M8">
-        <v>3.5075899452815098</v>
+        <v>3.2979367637975701</v>
       </c>
     </row>
   </sheetData>
@@ -1127,437 +1127,437 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
     </row>
     <row r="2" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <f>'copy raw data here'!E2</f>
-        <v>1.0521325881157999</v>
-      </c>
-      <c r="C3" s="9">
+        <v>1.01421166801854</v>
+      </c>
+      <c r="C3" s="8">
         <f>'copy raw data here'!F2</f>
-        <v>1.05135495334442</v>
-      </c>
-      <c r="D3" s="10">
+        <v>1.0566785240185399</v>
+      </c>
+      <c r="D3" s="9">
         <f>'copy raw data here'!G2</f>
-        <v>1.12663722334442</v>
-      </c>
-      <c r="E3" s="11">
+        <v>1.13210450601854</v>
+      </c>
+      <c r="E3" s="10">
         <f>'copy raw data here'!B2/100</f>
-        <v>0.11199999999999999</v>
-      </c>
-      <c r="F3" s="12">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F3" s="11">
         <f>'copy raw data here'!C2/100</f>
-        <v>-5.2999999999999999E-2</v>
-      </c>
-      <c r="G3" s="13">
+        <v>-0.11199999999999999</v>
+      </c>
+      <c r="G3" s="12">
         <f>'copy raw data here'!D2/100</f>
+        <v>0.433</v>
+      </c>
+      <c r="H3" s="13">
+        <f>'copy raw data here'!K2</f>
+        <v>3.1335955590101099</v>
+      </c>
+      <c r="I3" s="14">
+        <f>'copy raw data here'!L2</f>
+        <v>2.8449553227162201</v>
+      </c>
+      <c r="J3" s="14">
+        <f>'copy raw data here'!M2</f>
+        <v>2.8956860816209802</v>
+      </c>
+      <c r="K3" s="7">
+        <f>'copy raw data here'!H2</f>
+        <v>0.863922892747502</v>
+      </c>
+      <c r="L3" s="8">
+        <f>'copy raw data here'!I2</f>
+        <v>0.80795694980699195</v>
+      </c>
+      <c r="M3" s="9">
+        <f>'copy raw data here'!J2</f>
+        <v>0.65750235090564702</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="16">
+        <f>'copy raw data here'!E3</f>
+        <v>1.27413992293317</v>
+      </c>
+      <c r="C4" s="17">
+        <f>'copy raw data here'!F3</f>
+        <v>1.22370623293317</v>
+      </c>
+      <c r="D4" s="18">
+        <f>'copy raw data here'!G3</f>
+        <v>1.7079850700619399</v>
+      </c>
+      <c r="E4" s="19">
+        <f>'copy raw data here'!B3/100</f>
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="F4" s="20">
+        <f>'copy raw data here'!C3/100</f>
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="G4" s="21">
+        <f>'copy raw data here'!D3/100</f>
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="H4" s="22">
+        <f>'copy raw data here'!K3</f>
+        <v>4.0619192469853198</v>
+      </c>
+      <c r="I4" s="23">
+        <f>'copy raw data here'!L3</f>
+        <v>3.7149885047470099</v>
+      </c>
+      <c r="J4" s="23">
+        <f>'copy raw data here'!M3</f>
+        <v>3.73206031795227</v>
+      </c>
+      <c r="K4" s="16">
+        <f>'copy raw data here'!H3</f>
+        <v>0.96403640732375395</v>
+      </c>
+      <c r="L4" s="17">
+        <f>'copy raw data here'!I3</f>
+        <v>0.90247532090521798</v>
+      </c>
+      <c r="M4" s="18">
+        <f>'copy raw data here'!J3</f>
+        <v>0.83748434156848695</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="24">
+        <f>'copy raw data here'!E4</f>
+        <v>1.1513136169331699</v>
+      </c>
+      <c r="C5" s="25">
+        <f>'copy raw data here'!F4</f>
+        <v>0.98552670093317096</v>
+      </c>
+      <c r="D5" s="26">
+        <f>'copy raw data here'!G4</f>
+        <v>1.2129977769331699</v>
+      </c>
+      <c r="E5" s="27">
+        <f>'copy raw data here'!B4/100</f>
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="F5" s="28">
+        <f>'copy raw data here'!C4/100</f>
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="G5" s="29">
+        <f>'copy raw data here'!D4/100</f>
         <v>0.53</v>
       </c>
-      <c r="H3" s="14">
-        <f>'copy raw data here'!K2</f>
-        <v>3.3374783120993698</v>
-      </c>
-      <c r="I3" s="15">
-        <f>'copy raw data here'!L2</f>
-        <v>3.0269811296883899</v>
-      </c>
-      <c r="J3" s="15">
-        <f>'copy raw data here'!M2</f>
-        <v>3.0712426252462901</v>
-      </c>
-      <c r="K3" s="8">
-        <f>'copy raw data here'!H2</f>
-        <v>0.86376164822378598</v>
-      </c>
-      <c r="L3" s="9">
-        <f>'copy raw data here'!I2</f>
-        <v>0.80618789921720402</v>
-      </c>
-      <c r="M3" s="10">
-        <f>'copy raw data here'!J2</f>
-        <v>0.65203593676152205</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="17">
-        <f>'copy raw data here'!E3</f>
-        <v>1.3316947738145499</v>
-      </c>
-      <c r="C4" s="18">
-        <f>'copy raw data here'!F3</f>
-        <v>1.2724853541158001</v>
-      </c>
-      <c r="D4" s="19">
-        <f>'copy raw data here'!G3</f>
-        <v>1.83591235817483</v>
-      </c>
-      <c r="E4" s="20">
-        <f>'copy raw data here'!B3/100</f>
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="F4" s="21">
-        <f>'copy raw data here'!C3/100</f>
-        <v>0.45399999999999996</v>
-      </c>
-      <c r="G4" s="22">
-        <f>'copy raw data here'!D3/100</f>
-        <v>0.96499999999999997</v>
-      </c>
-      <c r="H4" s="23">
-        <f>'copy raw data here'!K3</f>
-        <v>4.3378172557114398</v>
-      </c>
-      <c r="I4" s="24">
-        <f>'copy raw data here'!L3</f>
-        <v>3.96624857761035</v>
-      </c>
-      <c r="J4" s="24">
-        <f>'copy raw data here'!M3</f>
-        <v>3.96295203219139</v>
-      </c>
-      <c r="K4" s="17">
-        <f>'copy raw data here'!H3</f>
-        <v>0.96907780717402503</v>
-      </c>
-      <c r="L4" s="18">
-        <f>'copy raw data here'!I3</f>
-        <v>0.90676330233740599</v>
-      </c>
-      <c r="M4" s="19">
-        <f>'copy raw data here'!J3</f>
-        <v>0.83250710429626895</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="25">
-        <f>'copy raw data here'!E4</f>
-        <v>1.2001283241158001</v>
-      </c>
-      <c r="C5" s="26">
-        <f>'copy raw data here'!F4</f>
-        <v>1.0342946601158001</v>
-      </c>
-      <c r="D5" s="27">
-        <f>'copy raw data here'!G4</f>
-        <v>1.3103127278145501</v>
-      </c>
-      <c r="E5" s="28">
-        <f>'copy raw data here'!B4/100</f>
-        <v>0.21600000000000003</v>
-      </c>
-      <c r="F5" s="29">
-        <f>'copy raw data here'!C4/100</f>
+      <c r="H5" s="30">
+        <f>'copy raw data here'!K4</f>
+        <v>3.6951717519075999</v>
+      </c>
+      <c r="I5" s="31">
+        <f>'copy raw data here'!L4</f>
+        <v>3.3400324767145899</v>
+      </c>
+      <c r="J5" s="31">
+        <f>'copy raw data here'!M4</f>
+        <v>3.4815001151263001</v>
+      </c>
+      <c r="K5" s="24">
+        <f>'copy raw data here'!H4</f>
+        <v>0.960542507354751</v>
+      </c>
+      <c r="L5" s="25">
+        <f>'copy raw data here'!I4</f>
+        <v>0.92077137459599301</v>
+      </c>
+      <c r="M5" s="26">
+        <f>'copy raw data here'!J4</f>
+        <v>0.85730046747484201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="16">
+        <f>'copy raw data here'!E5</f>
+        <v>1.1634389124664599</v>
+      </c>
+      <c r="C6" s="17">
+        <f>'copy raw data here'!F5</f>
+        <v>1.1978005744664599</v>
+      </c>
+      <c r="D6" s="18">
+        <f>'copy raw data here'!G5</f>
+        <v>1.23618700001854</v>
+      </c>
+      <c r="E6" s="19">
+        <f>'copy raw data here'!B5/100</f>
+        <v>-0.16699999999999998</v>
+      </c>
+      <c r="F6" s="20">
+        <f>'copy raw data here'!C5/100</f>
+        <v>-0.23699999999999999</v>
+      </c>
+      <c r="G6" s="21">
+        <f>'copy raw data here'!D5/100</f>
         <v>0.14099999999999999</v>
       </c>
-      <c r="G5" s="30">
-        <f>'copy raw data here'!D4/100</f>
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="H5" s="31">
-        <f>'copy raw data here'!K4</f>
-        <v>3.9460191028290601</v>
-      </c>
-      <c r="I5" s="32">
-        <f>'copy raw data here'!L4</f>
-        <v>3.5622311854927702</v>
-      </c>
-      <c r="J5" s="32">
-        <f>'copy raw data here'!M4</f>
-        <v>3.7016718989408801</v>
-      </c>
-      <c r="K5" s="25">
-        <f>'copy raw data here'!H4</f>
-        <v>0.96549445281805502</v>
-      </c>
-      <c r="L5" s="26">
-        <f>'copy raw data here'!I4</f>
-        <v>0.923217263031333</v>
-      </c>
-      <c r="M5" s="27">
-        <f>'copy raw data here'!J4</f>
-        <v>0.854431416194254</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="17">
-        <f>'copy raw data here'!E5</f>
-        <v>1.1044924468520101</v>
-      </c>
-      <c r="C6" s="18">
-        <f>'copy raw data here'!F5</f>
-        <v>1.1389014208520101</v>
-      </c>
-      <c r="D6" s="19">
-        <f>'copy raw data here'!G5</f>
-        <v>1.23074981734442</v>
-      </c>
-      <c r="E6" s="20">
-        <f>'copy raw data here'!B5/100</f>
-        <v>-0.111</v>
-      </c>
-      <c r="F6" s="21">
-        <f>'copy raw data here'!C5/100</f>
-        <v>-0.185</v>
-      </c>
-      <c r="G6" s="22">
-        <f>'copy raw data here'!D5/100</f>
-        <v>0.218</v>
-      </c>
-      <c r="H6" s="23">
+      <c r="H6" s="22">
         <f>'copy raw data here'!K5</f>
-        <v>3.57444354830821</v>
-      </c>
-      <c r="I6" s="24">
+        <v>3.34524192817543</v>
+      </c>
+      <c r="I6" s="23">
         <f>'copy raw data here'!L5</f>
-        <v>3.2202795644670599</v>
-      </c>
-      <c r="J6" s="24">
+        <v>3.0201145318680198</v>
+      </c>
+      <c r="J6" s="23">
         <f>'copy raw data here'!M5</f>
-        <v>3.91229008459465</v>
-      </c>
-      <c r="K6" s="17">
+        <v>3.6767724909794302</v>
+      </c>
+      <c r="K6" s="16">
         <f>'copy raw data here'!H5</f>
-        <v>0.894122469439247</v>
-      </c>
-      <c r="L6" s="18">
+        <v>0.88848660049837003</v>
+      </c>
+      <c r="L6" s="17">
         <f>'copy raw data here'!I5</f>
-        <v>0.83477331068213401</v>
-      </c>
-      <c r="M6" s="19">
+        <v>0.83297081032059195</v>
+      </c>
+      <c r="M6" s="18">
         <f>'copy raw data here'!J5</f>
-        <v>0.82944973105878195</v>
+        <v>0.83107424273178199</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="24">
         <f>'copy raw data here'!E6</f>
-        <v>1.1031031576234001</v>
-      </c>
-      <c r="C7" s="26">
+        <v>1.1078974873810801</v>
+      </c>
+      <c r="C7" s="25">
         <f>'copy raw data here'!F6</f>
-        <v>0.913943772852019</v>
-      </c>
-      <c r="D7" s="27">
+        <v>0.97308437046646201</v>
+      </c>
+      <c r="D7" s="26">
         <f>'copy raw data here'!G6</f>
-        <v>1.1440476861158</v>
-      </c>
-      <c r="E7" s="28">
+        <v>1.09541417093317</v>
+      </c>
+      <c r="E7" s="27">
         <f>'copy raw data here'!B6/100</f>
-        <v>0.10400000000000001</v>
-      </c>
-      <c r="F7" s="29">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="F7" s="28">
         <f>'copy raw data here'!C6/100</f>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G7" s="30">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="G7" s="29">
         <f>'copy raw data here'!D6/100</f>
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="H7" s="31">
+        <v>0.42100000000000004</v>
+      </c>
+      <c r="H7" s="30">
         <f>'copy raw data here'!K6</f>
-        <v>3.85586323818004</v>
-      </c>
-      <c r="I7" s="32">
+        <v>3.6110324960609801</v>
+      </c>
+      <c r="I7" s="31">
         <f>'copy raw data here'!L6</f>
-        <v>3.47859052554952</v>
-      </c>
-      <c r="J7" s="32">
+        <v>3.2626810758104599</v>
+      </c>
+      <c r="J7" s="31">
         <f>'copy raw data here'!M6</f>
-        <v>3.67247715845583</v>
-      </c>
-      <c r="K7" s="25">
+        <v>3.4540316842252601</v>
+      </c>
+      <c r="K7" s="24">
         <f>'copy raw data here'!H6</f>
-        <v>0.95321227213915605</v>
-      </c>
-      <c r="L7" s="26">
+        <v>0.948445807703301</v>
+      </c>
+      <c r="L7" s="25">
         <f>'copy raw data here'!I6</f>
-        <v>0.90836205052499497</v>
-      </c>
-      <c r="M7" s="27">
+        <v>0.90651028712940196</v>
+      </c>
+      <c r="M7" s="26">
         <f>'copy raw data here'!J6</f>
-        <v>0.82137053726634002</v>
+        <v>0.82402691999106004</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="16">
         <f>'copy raw data here'!E7</f>
-        <v>2.14756867017483</v>
-      </c>
-      <c r="C8" s="18">
+        <v>2.01920330806194</v>
+      </c>
+      <c r="C8" s="17">
         <f>'copy raw data here'!F7</f>
-        <v>1.76381402217483</v>
-      </c>
-      <c r="D8" s="19">
+        <v>1.6356503500619399</v>
+      </c>
+      <c r="D8" s="18">
         <f>'copy raw data here'!G7</f>
-        <v>3.01753937417483</v>
-      </c>
-      <c r="E8" s="20">
+        <v>2.88885652806194</v>
+      </c>
+      <c r="E8" s="19">
         <f>'copy raw data here'!B7/100</f>
-        <v>1.129</v>
-      </c>
-      <c r="F8" s="21">
+        <v>0.995</v>
+      </c>
+      <c r="F8" s="20">
         <f>'copy raw data here'!C7/100</f>
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="G8" s="22">
+        <v>0.80599999999999994</v>
+      </c>
+      <c r="G8" s="21">
         <f>'copy raw data here'!D7/100</f>
-        <v>1.5859999999999999</v>
-      </c>
-      <c r="H8" s="23">
+        <v>1.423</v>
+      </c>
+      <c r="H8" s="22">
         <f>'copy raw data here'!K7</f>
-        <v>3.6617285652198799</v>
-      </c>
-      <c r="I8" s="24">
+        <v>3.4311334422637598</v>
+      </c>
+      <c r="I8" s="23">
         <f>'copy raw data here'!L7</f>
-        <v>3.25056417293065</v>
-      </c>
-      <c r="J8" s="24">
+        <v>3.0480392336422102</v>
+      </c>
+      <c r="J8" s="23">
         <f>'copy raw data here'!M7</f>
-        <v>3.04284663926475</v>
-      </c>
-      <c r="K8" s="17">
+        <v>2.8587905302868402</v>
+      </c>
+      <c r="K8" s="16">
         <f>'copy raw data here'!H7</f>
-        <v>0.98516090863149497</v>
-      </c>
-      <c r="L8" s="18">
+        <v>0.98109238708060997</v>
+      </c>
+      <c r="L8" s="17">
         <f>'copy raw data here'!I7</f>
-        <v>0.94341262423966099</v>
-      </c>
-      <c r="M8" s="19">
+        <v>0.940742373788099</v>
+      </c>
+      <c r="M8" s="18">
         <f>'copy raw data here'!J7</f>
-        <v>0.79954221208533605</v>
+        <v>0.79998727147353899</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="34">
+      <c r="B9" s="33">
         <f>'copy raw data here'!E8</f>
-        <v>1.1344329836233999</v>
-      </c>
-      <c r="C9" s="35">
+        <v>1.13914671338108</v>
+      </c>
+      <c r="C9" s="34">
         <f>'copy raw data here'!F8</f>
-        <v>0.94102003762340003</v>
-      </c>
-      <c r="D9" s="36">
+        <v>0.94583763538108701</v>
+      </c>
+      <c r="D9" s="35">
         <f>'copy raw data here'!G8</f>
-        <v>1.0968711601158001</v>
-      </c>
-      <c r="E9" s="37">
+        <v>1.04815943493317</v>
+      </c>
+      <c r="E9" s="36">
         <f>'copy raw data here'!B8/100</f>
-        <v>-9.0000000000000011E-3</v>
-      </c>
-      <c r="F9" s="38">
+        <v>-7.0999999999999994E-2</v>
+      </c>
+      <c r="F9" s="37">
         <f>'copy raw data here'!C8/100</f>
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="G9" s="39">
+        <v>0.01</v>
+      </c>
+      <c r="G9" s="38">
         <f>'copy raw data here'!D8/100</f>
-        <v>0.36399999999999999</v>
-      </c>
-      <c r="H9" s="40">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="H9" s="39">
         <f>'copy raw data here'!K8</f>
-        <v>3.5464378974631199</v>
-      </c>
-      <c r="I9" s="41">
+        <v>3.3143642744465498</v>
+      </c>
+      <c r="I9" s="40">
         <f>'copy raw data here'!L8</f>
-        <v>3.4014070995100498</v>
-      </c>
-      <c r="J9" s="41">
+        <v>3.1830707103834901</v>
+      </c>
+      <c r="J9" s="40">
         <f>'copy raw data here'!M8</f>
-        <v>3.5075899452815098</v>
-      </c>
-      <c r="K9" s="34">
+        <v>3.2979367637975701</v>
+      </c>
+      <c r="K9" s="33">
         <f>'copy raw data here'!H8</f>
-        <v>0.94416586775407096</v>
-      </c>
-      <c r="L9" s="35">
+        <v>0.93563642400835201</v>
+      </c>
+      <c r="L9" s="34">
         <f>'copy raw data here'!I8</f>
-        <v>0.91687333267720295</v>
-      </c>
-      <c r="M9" s="36">
+        <v>0.91094405569218395</v>
+      </c>
+      <c r="M9" s="35">
         <f>'copy raw data here'!J8</f>
-        <v>0.89648646126581599</v>
+        <v>0.89904925620429799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update gridmet water year estimates; add radar precip estimates; inspect simple UID-PDIV matches
</commit_message>
<xml_diff>
--- a/figures+tables/Compare_OpenET-WIMAS_LEMA_allts_FitStats_Formatted.xlsx
+++ b/figures+tables/Compare_OpenET-WIMAS_LEMA_allts_FitStats_Formatted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s947z036\WorkGits\SD-6_MapWaterConservation\figures+tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCF9605-2439-4633-98C4-DC9720E9E804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220A59E3-5C72-4300-A969-CE93C2CED61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="copy raw data here" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Algorithm</t>
   </si>
@@ -200,6 +200,21 @@
       <t>2</t>
     </r>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Best in column</t>
+  </si>
+  <si>
+    <t>Best for metric</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Best average across algorithms</t>
+  </si>
 </sst>
 </file>
 
@@ -208,7 +223,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,8 +270,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +297,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,7 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -459,7 +514,6 @@
     <xf numFmtId="9" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -481,15 +535,41 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -774,7 +854,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="A1:XFD1048576"/>
+      <selection sqref="A1:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +911,7 @@
         <v>-11.2</v>
       </c>
       <c r="D2">
-        <v>43.3</v>
+        <v>5.3</v>
       </c>
       <c r="E2">
         <v>1.01421166801854</v>
@@ -840,7 +920,7 @@
         <v>1.0566785240185399</v>
       </c>
       <c r="G2">
-        <v>1.13210450601854</v>
+        <v>1.1525994500185399</v>
       </c>
       <c r="H2">
         <v>0.863922892747502</v>
@@ -849,7 +929,7 @@
         <v>0.80795694980699195</v>
       </c>
       <c r="J2">
-        <v>0.65750235090564702</v>
+        <v>0.67213203753411899</v>
       </c>
       <c r="K2">
         <v>3.1335955590101099</v>
@@ -858,7 +938,7 @@
         <v>2.8449553227162201</v>
       </c>
       <c r="M2">
-        <v>2.8956860816209802</v>
+        <v>2.6500996541601101</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -872,7 +952,7 @@
         <v>36.299999999999997</v>
       </c>
       <c r="D3">
-        <v>84.1</v>
+        <v>44.6</v>
       </c>
       <c r="E3">
         <v>1.27413992293317</v>
@@ -881,7 +961,7 @@
         <v>1.22370623293317</v>
       </c>
       <c r="G3">
-        <v>1.7079850700619399</v>
+        <v>1.4193805357288101</v>
       </c>
       <c r="H3">
         <v>0.96403640732375395</v>
@@ -890,7 +970,7 @@
         <v>0.90247532090521798</v>
       </c>
       <c r="J3">
-        <v>0.83748434156848695</v>
+        <v>0.86193462522872999</v>
       </c>
       <c r="K3">
         <v>4.0619192469853198</v>
@@ -899,7 +979,7 @@
         <v>3.7149885047470099</v>
       </c>
       <c r="M3">
-        <v>3.73206031795227</v>
+        <v>3.5658604898253898</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -913,7 +993,7 @@
         <v>6.9</v>
       </c>
       <c r="D4">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>1.1513136169331699</v>
@@ -922,7 +1002,7 @@
         <v>0.98552670093317096</v>
       </c>
       <c r="G4">
-        <v>1.2129977769331699</v>
+        <v>1.01319731893317</v>
       </c>
       <c r="H4">
         <v>0.960542507354751</v>
@@ -931,7 +1011,7 @@
         <v>0.92077137459599301</v>
       </c>
       <c r="J4">
-        <v>0.85730046747484201</v>
+        <v>0.88439845596157696</v>
       </c>
       <c r="K4">
         <v>3.6951717519075999</v>
@@ -940,7 +1020,7 @@
         <v>3.3400324767145899</v>
       </c>
       <c r="M4">
-        <v>3.4815001151263001</v>
+        <v>3.1024792559182002</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -954,7 +1034,7 @@
         <v>-23.7</v>
       </c>
       <c r="D5">
-        <v>14.1</v>
+        <v>-13.6</v>
       </c>
       <c r="E5">
         <v>1.1634389124664599</v>
@@ -963,7 +1043,7 @@
         <v>1.1978005744664599</v>
       </c>
       <c r="G5">
-        <v>1.23618700001854</v>
+        <v>1.0463966200185399</v>
       </c>
       <c r="H5">
         <v>0.88848660049837003</v>
@@ -972,7 +1052,7 @@
         <v>0.83297081032059195</v>
       </c>
       <c r="J5">
-        <v>0.83107424273178199</v>
+        <v>0.827581616833864</v>
       </c>
       <c r="K5">
         <v>3.34524192817543</v>
@@ -981,7 +1061,7 @@
         <v>3.0201145318680198</v>
       </c>
       <c r="M5">
-        <v>3.6767724909794302</v>
+        <v>2.8325471549336898</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -995,7 +1075,7 @@
         <v>-4.9000000000000004</v>
       </c>
       <c r="D6">
-        <v>42.1</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>1.1078974873810801</v>
@@ -1004,7 +1084,7 @@
         <v>0.97308437046646201</v>
       </c>
       <c r="G6">
-        <v>1.09541417093317</v>
+        <v>0.97808827601854598</v>
       </c>
       <c r="H6">
         <v>0.948445807703301</v>
@@ -1013,7 +1093,7 @@
         <v>0.90651028712940196</v>
       </c>
       <c r="J6">
-        <v>0.82402691999106004</v>
+        <v>0.87009602477077397</v>
       </c>
       <c r="K6">
         <v>3.6110324960609801</v>
@@ -1022,7 +1102,7 @@
         <v>3.2626810758104599</v>
       </c>
       <c r="M6">
-        <v>3.4540316842252601</v>
+        <v>3.0189485544990302</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1036,7 +1116,7 @@
         <v>80.599999999999994</v>
       </c>
       <c r="D7">
-        <v>142.30000000000001</v>
+        <v>91.4</v>
       </c>
       <c r="E7">
         <v>2.01920330806194</v>
@@ -1045,7 +1125,7 @@
         <v>1.6356503500619399</v>
       </c>
       <c r="G7">
-        <v>2.88885652806194</v>
+        <v>2.00649452772881</v>
       </c>
       <c r="H7">
         <v>0.98109238708060997</v>
@@ -1054,7 +1134,7 @@
         <v>0.940742373788099</v>
       </c>
       <c r="J7">
-        <v>0.79998727147353899</v>
+        <v>0.89024479358783104</v>
       </c>
       <c r="K7">
         <v>3.4311334422637598</v>
@@ -1063,7 +1143,7 @@
         <v>3.0480392336422102</v>
       </c>
       <c r="M7">
-        <v>2.8587905302868402</v>
+        <v>3.3774499167452801</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1077,7 +1157,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>27.8</v>
+        <v>-3.3</v>
       </c>
       <c r="E8">
         <v>1.13914671338108</v>
@@ -1086,7 +1166,7 @@
         <v>0.94583763538108701</v>
       </c>
       <c r="G8">
-        <v>1.04815943493317</v>
+        <v>0.79808015401854604</v>
       </c>
       <c r="H8">
         <v>0.93563642400835201</v>
@@ -1095,7 +1175,7 @@
         <v>0.91094405569218395</v>
       </c>
       <c r="J8">
-        <v>0.89904925620429799</v>
+        <v>0.90558260577088101</v>
       </c>
       <c r="K8">
         <v>3.3143642744465498</v>
@@ -1104,7 +1184,7 @@
         <v>3.1830707103834901</v>
       </c>
       <c r="M8">
-        <v>3.2979367637975701</v>
+        <v>2.63706430056543</v>
       </c>
     </row>
   </sheetData>
@@ -1114,41 +1194,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174954FC-3560-46B8-875C-4291803A546D}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
     </row>
-    <row r="2" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1189,11 +1270,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="47">
         <f>'copy raw data here'!E2</f>
         <v>1.01421166801854</v>
       </c>
@@ -1203,7 +1284,7 @@
       </c>
       <c r="D3" s="9">
         <f>'copy raw data here'!G2</f>
-        <v>1.13210450601854</v>
+        <v>1.1525994500185399</v>
       </c>
       <c r="E3" s="10">
         <f>'copy raw data here'!B2/100</f>
@@ -1215,19 +1296,19 @@
       </c>
       <c r="G3" s="12">
         <f>'copy raw data here'!D2/100</f>
-        <v>0.433</v>
-      </c>
-      <c r="H3" s="13">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="H3" s="52">
         <f>'copy raw data here'!K2</f>
         <v>3.1335955590101099</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="53">
         <f>'copy raw data here'!L2</f>
         <v>2.8449553227162201</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="13">
         <f>'copy raw data here'!M2</f>
-        <v>2.8956860816209802</v>
+        <v>2.6500996541601101</v>
       </c>
       <c r="K3" s="7">
         <f>'copy raw data here'!H2</f>
@@ -1239,325 +1320,390 @@
       </c>
       <c r="M3" s="9">
         <f>'copy raw data here'!J2</f>
-        <v>0.65750235090564702</v>
+        <v>0.67213203753411899</v>
+      </c>
+      <c r="N3" s="66" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="15">
         <f>'copy raw data here'!E3</f>
         <v>1.27413992293317</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="16">
         <f>'copy raw data here'!F3</f>
         <v>1.22370623293317</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <f>'copy raw data here'!G3</f>
-        <v>1.7079850700619399</v>
-      </c>
-      <c r="E4" s="19">
+        <v>1.4193805357288101</v>
+      </c>
+      <c r="E4" s="18">
         <f>'copy raw data here'!B3/100</f>
         <v>0.44900000000000001</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="19">
         <f>'copy raw data here'!C3/100</f>
         <v>0.36299999999999999</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="20">
         <f>'copy raw data here'!D3/100</f>
-        <v>0.84099999999999997</v>
-      </c>
-      <c r="H4" s="22">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="H4" s="21">
         <f>'copy raw data here'!K3</f>
         <v>4.0619192469853198</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="22">
         <f>'copy raw data here'!L3</f>
         <v>3.7149885047470099</v>
       </c>
-      <c r="J4" s="23">
+      <c r="J4" s="22">
         <f>'copy raw data here'!M3</f>
-        <v>3.73206031795227</v>
-      </c>
-      <c r="K4" s="16">
+        <v>3.5658604898253898</v>
+      </c>
+      <c r="K4" s="15">
         <f>'copy raw data here'!H3</f>
         <v>0.96403640732375395</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4" s="16">
         <f>'copy raw data here'!I3</f>
         <v>0.90247532090521798</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="17">
         <f>'copy raw data here'!J3</f>
-        <v>0.83748434156848695</v>
+        <v>0.86193462522872999</v>
+      </c>
+      <c r="N4" s="65" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <f>'copy raw data here'!E4</f>
         <v>1.1513136169331699</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="24">
         <f>'copy raw data here'!F4</f>
         <v>0.98552670093317096</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <f>'copy raw data here'!G4</f>
-        <v>1.2129977769331699</v>
-      </c>
-      <c r="E5" s="27">
+        <v>1.01319731893317</v>
+      </c>
+      <c r="E5" s="26">
         <f>'copy raw data here'!B4/100</f>
         <v>0.13900000000000001</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="27">
         <f>'copy raw data here'!C4/100</f>
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="28">
         <f>'copy raw data here'!D4/100</f>
-        <v>0.53</v>
-      </c>
-      <c r="H5" s="30">
+        <v>0.17</v>
+      </c>
+      <c r="H5" s="29">
         <f>'copy raw data here'!K4</f>
         <v>3.6951717519075999</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="30">
         <f>'copy raw data here'!L4</f>
         <v>3.3400324767145899</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="30">
         <f>'copy raw data here'!M4</f>
-        <v>3.4815001151263001</v>
-      </c>
-      <c r="K5" s="24">
+        <v>3.1024792559182002</v>
+      </c>
+      <c r="K5" s="23">
         <f>'copy raw data here'!H4</f>
         <v>0.960542507354751</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="24">
         <f>'copy raw data here'!I4</f>
         <v>0.92077137459599301</v>
       </c>
-      <c r="M5" s="26">
+      <c r="M5" s="25">
         <f>'copy raw data here'!J4</f>
-        <v>0.85730046747484201</v>
+        <v>0.88439845596157696</v>
+      </c>
+      <c r="N5" s="64" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="15">
         <f>'copy raw data here'!E5</f>
         <v>1.1634389124664599</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <f>'copy raw data here'!F5</f>
         <v>1.1978005744664599</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <f>'copy raw data here'!G5</f>
-        <v>1.23618700001854</v>
-      </c>
-      <c r="E6" s="19">
+        <v>1.0463966200185399</v>
+      </c>
+      <c r="E6" s="18">
         <f>'copy raw data here'!B5/100</f>
         <v>-0.16699999999999998</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="19">
         <f>'copy raw data here'!C5/100</f>
         <v>-0.23699999999999999</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="20">
         <f>'copy raw data here'!D5/100</f>
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="H6" s="22">
+        <v>-0.13600000000000001</v>
+      </c>
+      <c r="H6" s="21">
         <f>'copy raw data here'!K5</f>
         <v>3.34524192817543</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="22">
         <f>'copy raw data here'!L5</f>
         <v>3.0201145318680198</v>
       </c>
-      <c r="J6" s="23">
+      <c r="J6" s="22">
         <f>'copy raw data here'!M5</f>
-        <v>3.6767724909794302</v>
-      </c>
-      <c r="K6" s="16">
+        <v>2.8325471549336898</v>
+      </c>
+      <c r="K6" s="15">
         <f>'copy raw data here'!H5</f>
         <v>0.88848660049837003</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="16">
         <f>'copy raw data here'!I5</f>
         <v>0.83297081032059195</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="17">
         <f>'copy raw data here'!J5</f>
-        <v>0.83107424273178199</v>
+        <v>0.827581616833864</v>
+      </c>
+      <c r="N6" s="63" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <f>'copy raw data here'!E6</f>
         <v>1.1078974873810801</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="24">
         <f>'copy raw data here'!F6</f>
         <v>0.97308437046646201</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="25">
         <f>'copy raw data here'!G6</f>
-        <v>1.09541417093317</v>
-      </c>
-      <c r="E7" s="27">
+        <v>0.97808827601854598</v>
+      </c>
+      <c r="E7" s="50">
         <f>'copy raw data here'!B6/100</f>
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="27">
         <f>'copy raw data here'!C6/100</f>
         <v>-4.9000000000000002E-2</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="28">
         <f>'copy raw data here'!D6/100</f>
-        <v>0.42100000000000004</v>
-      </c>
-      <c r="H7" s="30">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H7" s="29">
         <f>'copy raw data here'!K6</f>
         <v>3.6110324960609801</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="30">
         <f>'copy raw data here'!L6</f>
         <v>3.2626810758104599</v>
       </c>
-      <c r="J7" s="31">
+      <c r="J7" s="30">
         <f>'copy raw data here'!M6</f>
-        <v>3.4540316842252601</v>
-      </c>
-      <c r="K7" s="24">
+        <v>3.0189485544990302</v>
+      </c>
+      <c r="K7" s="23">
         <f>'copy raw data here'!H6</f>
         <v>0.948445807703301</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="24">
         <f>'copy raw data here'!I6</f>
         <v>0.90651028712940196</v>
       </c>
-      <c r="M7" s="26">
+      <c r="M7" s="25">
         <f>'copy raw data here'!J6</f>
-        <v>0.82402691999106004</v>
+        <v>0.87009602477077397</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="15">
         <f>'copy raw data here'!E7</f>
         <v>2.01920330806194</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="16">
         <f>'copy raw data here'!F7</f>
         <v>1.6356503500619399</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <f>'copy raw data here'!G7</f>
-        <v>2.88885652806194</v>
-      </c>
-      <c r="E8" s="19">
+        <v>2.00649452772881</v>
+      </c>
+      <c r="E8" s="18">
         <f>'copy raw data here'!B7/100</f>
         <v>0.995</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="19">
         <f>'copy raw data here'!C7/100</f>
         <v>0.80599999999999994</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="20">
         <f>'copy raw data here'!D7/100</f>
-        <v>1.423</v>
-      </c>
-      <c r="H8" s="22">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="H8" s="21">
         <f>'copy raw data here'!K7</f>
         <v>3.4311334422637598</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="22">
         <f>'copy raw data here'!L7</f>
         <v>3.0480392336422102</v>
       </c>
-      <c r="J8" s="23">
+      <c r="J8" s="22">
         <f>'copy raw data here'!M7</f>
-        <v>2.8587905302868402</v>
-      </c>
-      <c r="K8" s="16">
+        <v>3.3774499167452801</v>
+      </c>
+      <c r="K8" s="58">
         <f>'copy raw data here'!H7</f>
         <v>0.98109238708060997</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="54">
         <f>'copy raw data here'!I7</f>
         <v>0.940742373788099</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="17">
         <f>'copy raw data here'!J7</f>
-        <v>0.79998727147353899</v>
+        <v>0.89024479358783104</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="32">
         <f>'copy raw data here'!E8</f>
         <v>1.13914671338108</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="48">
         <f>'copy raw data here'!F8</f>
         <v>0.94583763538108701</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="55">
         <f>'copy raw data here'!G8</f>
-        <v>1.04815943493317</v>
-      </c>
-      <c r="E9" s="36">
+        <v>0.79808015401854604</v>
+      </c>
+      <c r="E9" s="34">
         <f>'copy raw data here'!B8/100</f>
         <v>-7.0999999999999994E-2</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="56">
         <f>'copy raw data here'!C8/100</f>
         <v>0.01</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="51">
         <f>'copy raw data here'!D8/100</f>
-        <v>0.27800000000000002</v>
-      </c>
-      <c r="H9" s="39">
+        <v>-3.3000000000000002E-2</v>
+      </c>
+      <c r="H9" s="35">
         <f>'copy raw data here'!K8</f>
         <v>3.3143642744465498</v>
       </c>
-      <c r="I9" s="40">
+      <c r="I9" s="36">
         <f>'copy raw data here'!L8</f>
         <v>3.1830707103834901</v>
       </c>
-      <c r="J9" s="40">
+      <c r="J9" s="57">
         <f>'copy raw data here'!M8</f>
-        <v>3.2979367637975701</v>
-      </c>
-      <c r="K9" s="33">
+        <v>2.63706430056543</v>
+      </c>
+      <c r="K9" s="32">
         <f>'copy raw data here'!H8</f>
         <v>0.93563642400835201</v>
       </c>
-      <c r="L9" s="34">
+      <c r="L9" s="33">
         <f>'copy raw data here'!I8</f>
         <v>0.91094405569218395</v>
       </c>
-      <c r="M9" s="35">
+      <c r="M9" s="49">
         <f>'copy raw data here'!J8</f>
-        <v>0.89904925620429799</v>
+        <v>0.90558260577088101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="42">
+        <f>AVERAGE(B3:B9)</f>
+        <v>1.2670502327393487</v>
+      </c>
+      <c r="C10" s="59">
+        <f t="shared" ref="C10:M10" si="0">AVERAGE(C3:C9)</f>
+        <v>1.1454691983229759</v>
+      </c>
+      <c r="D10" s="39">
+        <f t="shared" si="0"/>
+        <v>1.2020338403521376</v>
+      </c>
+      <c r="E10" s="46">
+        <f t="shared" si="0"/>
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="F10" s="60">
+        <f t="shared" si="0"/>
+        <v>0.12142857142857143</v>
+      </c>
+      <c r="G10" s="40">
+        <f t="shared" si="0"/>
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="H10" s="45">
+        <f t="shared" si="0"/>
+        <v>3.5132083855499645</v>
+      </c>
+      <c r="I10" s="41">
+        <f t="shared" si="0"/>
+        <v>3.2019831222688571</v>
+      </c>
+      <c r="J10" s="61">
+        <f t="shared" si="0"/>
+        <v>3.0263499038067327</v>
+      </c>
+      <c r="K10" s="62">
+        <f t="shared" si="0"/>
+        <v>0.93459471810237704</v>
+      </c>
+      <c r="L10" s="43">
+        <f t="shared" si="0"/>
+        <v>0.88891016746264007</v>
+      </c>
+      <c r="M10" s="44">
+        <f t="shared" si="0"/>
+        <v>0.84456716566968226</v>
       </c>
     </row>
   </sheetData>
@@ -1568,5 +1714,6 @@
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add precipitation adjustment calculations
</commit_message>
<xml_diff>
--- a/figures+tables/Compare_OpenET-WIMAS_LEMA_allts_FitStats_Formatted.xlsx
+++ b/figures+tables/Compare_OpenET-WIMAS_LEMA_allts_FitStats_Formatted.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s947z036\WorkGits\SD-6_MapWaterConservation\figures+tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220A59E3-5C72-4300-A969-CE93C2CED61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185FF389-D804-4AD0-BCE4-75615EC9A552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="copy raw data here" sheetId="1" r:id="rId1"/>
-    <sheet name="Formatted table" sheetId="3" r:id="rId2"/>
+    <sheet name="Table 1 formatted" sheetId="3" r:id="rId2"/>
+    <sheet name="Table S1 Precip corrected table" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Algorithm</t>
   </si>
@@ -215,13 +216,17 @@
   <si>
     <t>Best average across algorithms</t>
   </si>
+  <si>
+    <t>Model</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -494,7 +499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -570,6 +575,28 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1196,8 +1223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174954FC-3560-46B8-875C-4291803A546D}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,30 +1235,30 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37" t="s">
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37" t="s">
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37" t="s">
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
     </row>
     <row r="2" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>17</v>
@@ -1716,4 +1743,161 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926FA25B-0675-4415-9EAE-A1DBC10ABC93}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="A1:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="5" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="69"/>
+      <c r="G1" s="68"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="72">
+        <v>7.9843275851626205E-2</v>
+      </c>
+      <c r="C2" s="73">
+        <v>0</v>
+      </c>
+      <c r="D2" s="74">
+        <v>0.96608893313863597</v>
+      </c>
+      <c r="E2" s="75">
+        <v>0.95567648290093599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="76">
+        <v>0.33006284778181</v>
+      </c>
+      <c r="C3" s="73">
+        <v>0</v>
+      </c>
+      <c r="D3" s="75">
+        <v>0.50274477265071404</v>
+      </c>
+      <c r="E3" s="75">
+        <v>0.81607488413903095</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="76">
+        <v>0.11268165096900799</v>
+      </c>
+      <c r="C4" s="73">
+        <v>0</v>
+      </c>
+      <c r="D4" s="75">
+        <v>0.92275076563106995</v>
+      </c>
+      <c r="E4" s="75">
+        <v>0.92177564416106395</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="76">
+        <v>0.24973661778678599</v>
+      </c>
+      <c r="C5" s="73">
+        <v>0</v>
+      </c>
+      <c r="D5" s="75">
+        <v>0.65056524434603202</v>
+      </c>
+      <c r="E5" s="75">
+        <v>0.80530314534528502</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="72">
+        <v>9.9349474711792798E-2</v>
+      </c>
+      <c r="C6" s="73">
+        <v>0</v>
+      </c>
+      <c r="D6" s="75">
+        <v>0.930632854423041</v>
+      </c>
+      <c r="E6" s="75">
+        <v>0.926004138245069</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="72">
+        <v>1.9286508155455399E-2</v>
+      </c>
+      <c r="C7" s="73">
+        <v>0</v>
+      </c>
+      <c r="D7" s="75">
+        <v>0.99793938228183798</v>
+      </c>
+      <c r="E7" s="75">
+        <v>0.98823072217984298</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="76">
+        <v>0.14938623912125501</v>
+      </c>
+      <c r="C8" s="73">
+        <v>0</v>
+      </c>
+      <c r="D8" s="75">
+        <v>0.88398014198517305</v>
+      </c>
+      <c r="E8" s="75">
+        <v>0.94584528914719102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
More updates to Peff calculations
</commit_message>
<xml_diff>
--- a/figures+tables/Compare_OpenET-WIMAS_LEMA_allts_FitStats_Formatted.xlsx
+++ b/figures+tables/Compare_OpenET-WIMAS_LEMA_allts_FitStats_Formatted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s947z036\WorkGits\SD-6_MapWaterConservation\figures+tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9447FF5F-BBCE-42C9-8E89-6F39C9D5FCB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A9C289-1D70-4036-B303-BAB193253A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 - copy raw data here" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="49">
   <si>
     <t>Algorithm</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>MAE_1e7m3</t>
+  </si>
+  <si>
+    <t>Calendar Year</t>
   </si>
 </sst>
 </file>
@@ -319,7 +322,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,12 +332,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,7 +523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -567,27 +564,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -604,16 +591,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -694,8 +672,28 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -984,6 +982,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1031,40 +1033,40 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>4.2</v>
+        <v>65.400000000000006</v>
       </c>
       <c r="C2">
-        <v>-11.2</v>
+        <v>46.8</v>
       </c>
       <c r="D2">
-        <v>5.3</v>
+        <v>50.6</v>
       </c>
       <c r="E2">
-        <v>1.01421166801854</v>
+        <v>1.3264925760619399</v>
       </c>
       <c r="F2">
-        <v>1.0566785240185399</v>
+        <v>0.94977537606193996</v>
       </c>
       <c r="G2">
-        <v>1.1525994500185399</v>
+        <v>1.1936025751473101</v>
       </c>
       <c r="H2">
-        <v>0.863922892747502</v>
+        <v>0.70722325678104503</v>
       </c>
       <c r="I2">
-        <v>0.80795694980699195</v>
+        <v>0.69082503808143803</v>
       </c>
       <c r="J2">
-        <v>0.67213203753411899</v>
+        <v>0.31761842437134202</v>
       </c>
       <c r="K2">
-        <v>0.27569699933465902</v>
+        <v>0.40690748489495798</v>
       </c>
       <c r="L2">
-        <v>0.28399635781822902</v>
+        <v>0.43274806461895099</v>
       </c>
       <c r="M2">
-        <v>0.253625193482445</v>
+        <v>0.22662206988995201</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1072,40 +1074,40 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>44.9</v>
+        <v>108.6</v>
       </c>
       <c r="C3">
-        <v>36.299999999999997</v>
+        <v>98.5</v>
       </c>
       <c r="D3">
-        <v>44.6</v>
+        <v>91.5</v>
       </c>
       <c r="E3">
-        <v>1.27413992293317</v>
+        <v>2.2049506480619399</v>
       </c>
       <c r="F3">
-        <v>1.22370623293317</v>
+        <v>2.00024414806194</v>
       </c>
       <c r="G3">
-        <v>1.4193805357288101</v>
+        <v>1.85773088406194</v>
       </c>
       <c r="H3">
-        <v>0.96403640732375395</v>
+        <v>0.96546512071329205</v>
       </c>
       <c r="I3">
-        <v>0.90247532090521798</v>
+        <v>0.87769876929967305</v>
       </c>
       <c r="J3">
-        <v>0.86193462522872999</v>
+        <v>0.63712450373597496</v>
       </c>
       <c r="K3">
-        <v>0.23733519765052999</v>
+        <v>0.377574803193928</v>
       </c>
       <c r="L3">
-        <v>0.242928159737785</v>
+        <v>0.38775196783792598</v>
       </c>
       <c r="M3">
-        <v>0.24171854947441701</v>
+        <v>0.28503364673370002</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1113,40 +1115,40 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>13.9</v>
+        <v>75</v>
       </c>
       <c r="C4">
-        <v>6.9</v>
+        <v>67.5</v>
       </c>
       <c r="D4">
-        <v>17</v>
+        <v>60.2</v>
       </c>
       <c r="E4">
-        <v>1.1513136169331699</v>
+        <v>1.5220841060619399</v>
       </c>
       <c r="F4">
-        <v>0.98552670093317096</v>
+        <v>1.3702253440619401</v>
       </c>
       <c r="G4">
-        <v>1.01319731893317</v>
+        <v>1.2227832780619401</v>
       </c>
       <c r="H4">
-        <v>0.960542507354751</v>
+        <v>0.98047507399070599</v>
       </c>
       <c r="I4">
-        <v>0.92077137459599301</v>
+        <v>0.93019406011203898</v>
       </c>
       <c r="J4">
-        <v>0.88439845596157696</v>
+        <v>0.67053346789159896</v>
       </c>
       <c r="K4">
-        <v>0.25994529397960398</v>
+        <v>0.41951285242667402</v>
       </c>
       <c r="L4">
-        <v>0.27567737170678802</v>
+        <v>0.46811426299519598</v>
       </c>
       <c r="M4">
-        <v>0.285061843451337</v>
+        <v>0.33694581169332799</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1154,40 +1156,40 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>-16.7</v>
+        <v>30.1</v>
       </c>
       <c r="C5">
-        <v>-23.7</v>
+        <v>25.4</v>
       </c>
       <c r="D5">
-        <v>-13.6</v>
+        <v>18.8</v>
       </c>
       <c r="E5">
-        <v>1.1634389124664599</v>
+        <v>0.83586382093317102</v>
       </c>
       <c r="F5">
-        <v>1.1978005744664599</v>
+        <v>0.60332796572881597</v>
       </c>
       <c r="G5">
-        <v>1.0463966200185399</v>
+        <v>0.88872024081419099</v>
       </c>
       <c r="H5">
-        <v>0.88848660049837003</v>
+        <v>0.95987013370315999</v>
       </c>
       <c r="I5">
-        <v>0.83297081032059195</v>
+        <v>0.88673729685160996</v>
       </c>
       <c r="J5">
-        <v>0.827581616833864</v>
+        <v>0.71027998243946699</v>
       </c>
       <c r="K5">
-        <v>0.265597113624295</v>
+        <v>0.35680908719869198</v>
       </c>
       <c r="L5">
-        <v>0.27580768925520699</v>
+        <v>0.39691877484075699</v>
       </c>
       <c r="M5">
-        <v>0.29216869890140901</v>
+        <v>0.30625140776853899</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1195,40 +1197,40 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>3.4</v>
+        <v>63</v>
       </c>
       <c r="C6">
-        <v>-4.9000000000000004</v>
+        <v>54.8</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>49.4</v>
       </c>
       <c r="E6">
-        <v>1.1078974873810801</v>
+        <v>1.2791523360619399</v>
       </c>
       <c r="F6">
-        <v>0.97308437046646201</v>
+        <v>1.11282718006194</v>
       </c>
       <c r="G6">
-        <v>0.97808827601854598</v>
+        <v>1.0036873200619401</v>
       </c>
       <c r="H6">
-        <v>0.948445807703301</v>
+        <v>0.97827409490972295</v>
       </c>
       <c r="I6">
-        <v>0.90651028712940096</v>
+        <v>0.91565097784484495</v>
       </c>
       <c r="J6">
-        <v>0.87009602477077397</v>
+        <v>0.64345323564458301</v>
       </c>
       <c r="K6">
-        <v>0.26265224938792198</v>
+        <v>0.417700106510139</v>
       </c>
       <c r="L6">
-        <v>0.27784213843340999</v>
+        <v>0.46456133905040398</v>
       </c>
       <c r="M6">
-        <v>0.28821161045427501</v>
+        <v>0.32831283047439103</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1236,40 +1238,40 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>99.5</v>
+        <v>165.6</v>
       </c>
       <c r="C7">
-        <v>80.599999999999994</v>
+        <v>144.4</v>
       </c>
       <c r="D7">
-        <v>91.4</v>
+        <v>149.9</v>
       </c>
       <c r="E7">
-        <v>2.01920330806194</v>
+        <v>3.3609131600619402</v>
       </c>
       <c r="F7">
-        <v>1.6356503500619399</v>
+        <v>2.9305214960619401</v>
       </c>
       <c r="G7">
-        <v>2.00649452772881</v>
+        <v>3.0432672320619401</v>
       </c>
       <c r="H7">
-        <v>0.98109238708060997</v>
+        <v>0.98400599280103296</v>
       </c>
       <c r="I7">
-        <v>0.940742373788099</v>
+        <v>0.93078577029168597</v>
       </c>
       <c r="J7">
-        <v>0.89024479358783104</v>
+        <v>0.568102088811406</v>
       </c>
       <c r="K7">
-        <v>0.285938277711901</v>
+        <v>0.54931383902197095</v>
       </c>
       <c r="L7">
-        <v>0.308638538311716</v>
+        <v>0.60926055216130204</v>
       </c>
       <c r="M7">
-        <v>0.26358489852773997</v>
+        <v>0.42013696880208601</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1277,40 +1279,40 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>-7.1</v>
+        <v>48.7</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>60.5</v>
       </c>
       <c r="D8">
-        <v>-3.3</v>
+        <v>33.9</v>
       </c>
       <c r="E8">
-        <v>1.13914671338108</v>
+        <v>0.98815472206193999</v>
       </c>
       <c r="F8">
-        <v>0.94583763538108701</v>
+        <v>1.2283358760619401</v>
       </c>
       <c r="G8">
-        <v>0.79808015401854604</v>
+        <v>0.86337590372881601</v>
       </c>
       <c r="H8">
-        <v>0.93563642400835201</v>
+        <v>0.96972039389537301</v>
       </c>
       <c r="I8">
-        <v>0.91094405569218295</v>
+        <v>0.90988591409012798</v>
       </c>
       <c r="J8">
-        <v>0.90558260577088101</v>
+        <v>0.69401816999657095</v>
       </c>
       <c r="K8">
-        <v>0.28229740201522902</v>
+        <v>0.441917209407449</v>
       </c>
       <c r="L8">
-        <v>0.28618404634260602</v>
+        <v>0.48907248286788402</v>
       </c>
       <c r="M8">
-        <v>0.34340558384439301</v>
+        <v>0.37111742539425402</v>
       </c>
     </row>
   </sheetData>
@@ -1322,45 +1324,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174954FC-3560-46B8-875C-4291803A546D}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
     <col min="14" max="14" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61" t="s">
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61" t="s">
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61" t="s">
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
     </row>
     <row r="2" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>18</v>
@@ -1369,7 +1375,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>18</v>
@@ -1378,7 +1384,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>18</v>
@@ -1387,7 +1393,7 @@
         <v>19</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>18</v>
@@ -1400,55 +1406,55 @@
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="7">
         <f>'Table 1 - copy raw data here'!E2</f>
-        <v>1.01421166801854</v>
+        <v>1.3264925760619399</v>
       </c>
       <c r="C3" s="8">
         <f>'Table 1 - copy raw data here'!F2</f>
-        <v>1.0566785240185399</v>
+        <v>0.94977537606193996</v>
       </c>
       <c r="D3" s="9">
         <f>'Table 1 - copy raw data here'!G2</f>
-        <v>1.1525994500185399</v>
+        <v>1.1936025751473101</v>
       </c>
       <c r="E3" s="10">
         <f>'Table 1 - copy raw data here'!B2/100</f>
-        <v>4.2000000000000003E-2</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="F3" s="11">
         <f>'Table 1 - copy raw data here'!C2/100</f>
-        <v>-0.11199999999999999</v>
+        <v>0.46799999999999997</v>
       </c>
       <c r="G3" s="12">
         <f>'Table 1 - copy raw data here'!D2/100</f>
-        <v>5.2999999999999999E-2</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="H3" s="7">
         <f>'Table 1 - copy raw data here'!K2</f>
-        <v>0.27569699933465902</v>
+        <v>0.40690748489495798</v>
       </c>
       <c r="I3" s="8">
         <f>'Table 1 - copy raw data here'!L2</f>
-        <v>0.28399635781822902</v>
+        <v>0.43274806461895099</v>
       </c>
       <c r="J3" s="8">
         <f>'Table 1 - copy raw data here'!M2</f>
-        <v>0.253625193482445</v>
+        <v>0.22662206988995201</v>
       </c>
       <c r="K3" s="7">
         <f>'Table 1 - copy raw data here'!H2</f>
-        <v>0.863922892747502</v>
+        <v>0.70722325678104503</v>
       </c>
       <c r="L3" s="8">
         <f>'Table 1 - copy raw data here'!I2</f>
-        <v>0.80795694980699195</v>
+        <v>0.69082503808143803</v>
       </c>
       <c r="M3" s="9">
         <f>'Table 1 - copy raw data here'!J2</f>
-        <v>0.67213203753411899</v>
-      </c>
-      <c r="N3" s="53" t="s">
+        <v>0.31761842437134202</v>
+      </c>
+      <c r="N3" s="43" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1458,53 +1464,53 @@
       </c>
       <c r="B4" s="14">
         <f>'Table 1 - copy raw data here'!E3</f>
-        <v>1.27413992293317</v>
+        <v>2.2049506480619399</v>
       </c>
       <c r="C4" s="15">
         <f>'Table 1 - copy raw data here'!F3</f>
-        <v>1.22370623293317</v>
+        <v>2.00024414806194</v>
       </c>
       <c r="D4" s="16">
         <f>'Table 1 - copy raw data here'!G3</f>
-        <v>1.4193805357288101</v>
+        <v>1.85773088406194</v>
       </c>
       <c r="E4" s="17">
         <f>'Table 1 - copy raw data here'!B3/100</f>
-        <v>0.44900000000000001</v>
+        <v>1.0859999999999999</v>
       </c>
       <c r="F4" s="18">
         <f>'Table 1 - copy raw data here'!C3/100</f>
-        <v>0.36299999999999999</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="G4" s="19">
         <f>'Table 1 - copy raw data here'!D3/100</f>
-        <v>0.44600000000000001</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="H4" s="14">
         <f>'Table 1 - copy raw data here'!K3</f>
-        <v>0.23733519765052999</v>
+        <v>0.377574803193928</v>
       </c>
       <c r="I4" s="15">
         <f>'Table 1 - copy raw data here'!L3</f>
-        <v>0.242928159737785</v>
+        <v>0.38775196783792598</v>
       </c>
       <c r="J4" s="15">
         <f>'Table 1 - copy raw data here'!M3</f>
-        <v>0.24171854947441701</v>
+        <v>0.28503364673370002</v>
       </c>
       <c r="K4" s="14">
         <f>'Table 1 - copy raw data here'!H3</f>
-        <v>0.96403640732375395</v>
+        <v>0.96546512071329205</v>
       </c>
       <c r="L4" s="15">
         <f>'Table 1 - copy raw data here'!I3</f>
-        <v>0.90247532090521798</v>
+        <v>0.87769876929967305</v>
       </c>
       <c r="M4" s="16">
         <f>'Table 1 - copy raw data here'!J3</f>
-        <v>0.86193462522872999</v>
-      </c>
-      <c r="N4" s="52" t="s">
+        <v>0.63712450373597496</v>
+      </c>
+      <c r="N4" s="42" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1514,53 +1520,53 @@
       </c>
       <c r="B5" s="20">
         <f>'Table 1 - copy raw data here'!E4</f>
-        <v>1.1513136169331699</v>
+        <v>1.5220841060619399</v>
       </c>
       <c r="C5" s="21">
         <f>'Table 1 - copy raw data here'!F4</f>
-        <v>0.98552670093317096</v>
+        <v>1.3702253440619401</v>
       </c>
       <c r="D5" s="22">
         <f>'Table 1 - copy raw data here'!G4</f>
-        <v>1.01319731893317</v>
+        <v>1.2227832780619401</v>
       </c>
       <c r="E5" s="23">
         <f>'Table 1 - copy raw data here'!B4/100</f>
-        <v>0.13900000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="F5" s="24">
         <f>'Table 1 - copy raw data here'!C4/100</f>
-        <v>6.9000000000000006E-2</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="G5" s="25">
         <f>'Table 1 - copy raw data here'!D4/100</f>
-        <v>0.17</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="H5" s="20">
         <f>'Table 1 - copy raw data here'!K4</f>
-        <v>0.25994529397960398</v>
+        <v>0.41951285242667402</v>
       </c>
       <c r="I5" s="21">
         <f>'Table 1 - copy raw data here'!L4</f>
-        <v>0.27567737170678802</v>
+        <v>0.46811426299519598</v>
       </c>
       <c r="J5" s="21">
         <f>'Table 1 - copy raw data here'!M4</f>
-        <v>0.285061843451337</v>
-      </c>
-      <c r="K5" s="20">
+        <v>0.33694581169332799</v>
+      </c>
+      <c r="K5" s="36">
         <f>'Table 1 - copy raw data here'!H4</f>
-        <v>0.960542507354751</v>
-      </c>
-      <c r="L5" s="21">
+        <v>0.98047507399070599</v>
+      </c>
+      <c r="L5" s="94">
         <f>'Table 1 - copy raw data here'!I4</f>
-        <v>0.92077137459599301</v>
+        <v>0.93019406011203898</v>
       </c>
       <c r="M5" s="22">
         <f>'Table 1 - copy raw data here'!J4</f>
-        <v>0.88439845596157696</v>
-      </c>
-      <c r="N5" s="51" t="s">
+        <v>0.67053346789159896</v>
+      </c>
+      <c r="N5" s="41" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1568,55 +1574,55 @@
       <c r="A6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="88">
         <f>'Table 1 - copy raw data here'!E5</f>
-        <v>1.1634389124664599</v>
-      </c>
-      <c r="C6" s="15">
+        <v>0.83586382093317102</v>
+      </c>
+      <c r="C6" s="89">
         <f>'Table 1 - copy raw data here'!F5</f>
-        <v>1.1978005744664599</v>
+        <v>0.60332796572881597</v>
       </c>
       <c r="D6" s="16">
         <f>'Table 1 - copy raw data here'!G5</f>
-        <v>1.0463966200185399</v>
-      </c>
-      <c r="E6" s="17">
+        <v>0.88872024081419099</v>
+      </c>
+      <c r="E6" s="91">
         <f>'Table 1 - copy raw data here'!B5/100</f>
-        <v>-0.16699999999999998</v>
-      </c>
-      <c r="F6" s="18">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="F6" s="92">
         <f>'Table 1 - copy raw data here'!C5/100</f>
-        <v>-0.23699999999999999</v>
-      </c>
-      <c r="G6" s="19">
+        <v>0.254</v>
+      </c>
+      <c r="G6" s="93">
         <f>'Table 1 - copy raw data here'!D5/100</f>
-        <v>-0.13600000000000001</v>
+        <v>0.188</v>
       </c>
       <c r="H6" s="14">
         <f>'Table 1 - copy raw data here'!K5</f>
-        <v>0.265597113624295</v>
+        <v>0.35680908719869198</v>
       </c>
       <c r="I6" s="15">
         <f>'Table 1 - copy raw data here'!L5</f>
-        <v>0.27580768925520699</v>
+        <v>0.39691877484075699</v>
       </c>
       <c r="J6" s="15">
         <f>'Table 1 - copy raw data here'!M5</f>
-        <v>0.29216869890140901</v>
+        <v>0.30625140776853899</v>
       </c>
       <c r="K6" s="14">
         <f>'Table 1 - copy raw data here'!H5</f>
-        <v>0.88848660049837003</v>
+        <v>0.95987013370315999</v>
       </c>
       <c r="L6" s="15">
         <f>'Table 1 - copy raw data here'!I5</f>
-        <v>0.83297081032059195</v>
-      </c>
-      <c r="M6" s="16">
+        <v>0.88673729685160996</v>
+      </c>
+      <c r="M6" s="95">
         <f>'Table 1 - copy raw data here'!J5</f>
-        <v>0.827581616833864</v>
-      </c>
-      <c r="N6" s="50" t="s">
+        <v>0.71027998243946699</v>
+      </c>
+      <c r="N6" s="40" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1626,51 +1632,51 @@
       </c>
       <c r="B7" s="20">
         <f>'Table 1 - copy raw data here'!E6</f>
-        <v>1.1078974873810801</v>
+        <v>1.2791523360619399</v>
       </c>
       <c r="C7" s="21">
         <f>'Table 1 - copy raw data here'!F6</f>
-        <v>0.97308437046646201</v>
+        <v>1.11282718006194</v>
       </c>
       <c r="D7" s="22">
         <f>'Table 1 - copy raw data here'!G6</f>
-        <v>0.97808827601854598</v>
-      </c>
-      <c r="E7" s="41">
+        <v>1.0036873200619401</v>
+      </c>
+      <c r="E7" s="23">
         <f>'Table 1 - copy raw data here'!B6/100</f>
-        <v>3.4000000000000002E-2</v>
+        <v>0.63</v>
       </c>
       <c r="F7" s="24">
         <f>'Table 1 - copy raw data here'!C6/100</f>
-        <v>-4.9000000000000002E-2</v>
+        <v>0.54799999999999993</v>
       </c>
       <c r="G7" s="25">
         <f>'Table 1 - copy raw data here'!D6/100</f>
-        <v>7.0000000000000007E-2</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="H7" s="20">
         <f>'Table 1 - copy raw data here'!K6</f>
-        <v>0.26265224938792198</v>
+        <v>0.417700106510139</v>
       </c>
       <c r="I7" s="21">
         <f>'Table 1 - copy raw data here'!L6</f>
-        <v>0.27784213843340999</v>
+        <v>0.46456133905040398</v>
       </c>
       <c r="J7" s="21">
         <f>'Table 1 - copy raw data here'!M6</f>
-        <v>0.28821161045427501</v>
-      </c>
-      <c r="K7" s="20">
+        <v>0.32831283047439103</v>
+      </c>
+      <c r="K7" s="36">
         <f>'Table 1 - copy raw data here'!H6</f>
-        <v>0.948445807703301</v>
+        <v>0.97827409490972295</v>
       </c>
       <c r="L7" s="21">
         <f>'Table 1 - copy raw data here'!I6</f>
-        <v>0.90651028712940096</v>
+        <v>0.91565097784484495</v>
       </c>
       <c r="M7" s="22">
         <f>'Table 1 - copy raw data here'!J6</f>
-        <v>0.87009602477077397</v>
+        <v>0.64345323564458301</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1679,51 +1685,51 @@
       </c>
       <c r="B8" s="14">
         <f>'Table 1 - copy raw data here'!E7</f>
-        <v>2.01920330806194</v>
+        <v>3.3609131600619402</v>
       </c>
       <c r="C8" s="15">
         <f>'Table 1 - copy raw data here'!F7</f>
-        <v>1.6356503500619399</v>
+        <v>2.9305214960619401</v>
       </c>
       <c r="D8" s="16">
         <f>'Table 1 - copy raw data here'!G7</f>
-        <v>2.00649452772881</v>
+        <v>3.0432672320619401</v>
       </c>
       <c r="E8" s="17">
         <f>'Table 1 - copy raw data here'!B7/100</f>
-        <v>0.995</v>
+        <v>1.6559999999999999</v>
       </c>
       <c r="F8" s="18">
         <f>'Table 1 - copy raw data here'!C7/100</f>
-        <v>0.80599999999999994</v>
+        <v>1.444</v>
       </c>
       <c r="G8" s="19">
         <f>'Table 1 - copy raw data here'!D7/100</f>
-        <v>0.91400000000000003</v>
-      </c>
-      <c r="H8" s="94">
+        <v>1.4990000000000001</v>
+      </c>
+      <c r="H8" s="88">
         <f>'Table 1 - copy raw data here'!K7</f>
-        <v>0.285938277711901</v>
-      </c>
-      <c r="I8" s="43">
+        <v>0.54931383902197095</v>
+      </c>
+      <c r="I8" s="89">
         <f>'Table 1 - copy raw data here'!L7</f>
-        <v>0.308638538311716</v>
-      </c>
-      <c r="J8" s="15">
+        <v>0.60926055216130204</v>
+      </c>
+      <c r="J8" s="94">
         <f>'Table 1 - copy raw data here'!M7</f>
-        <v>0.26358489852773997</v>
-      </c>
-      <c r="K8" s="46">
+        <v>0.42013696880208601</v>
+      </c>
+      <c r="K8" s="36">
         <f>'Table 1 - copy raw data here'!H7</f>
-        <v>0.98109238708060997</v>
-      </c>
-      <c r="L8" s="43">
+        <v>0.98400599280103296</v>
+      </c>
+      <c r="L8" s="94">
         <f>'Table 1 - copy raw data here'!I7</f>
-        <v>0.940742373788099</v>
+        <v>0.93078577029168597</v>
       </c>
       <c r="M8" s="16">
         <f>'Table 1 - copy raw data here'!J7</f>
-        <v>0.89024479358783104</v>
+        <v>0.568102088811406</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1732,104 +1738,104 @@
       </c>
       <c r="B9" s="27">
         <f>'Table 1 - copy raw data here'!E8</f>
-        <v>1.13914671338108</v>
-      </c>
-      <c r="C9" s="39">
+        <v>0.98815472206193999</v>
+      </c>
+      <c r="C9" s="28">
         <f>'Table 1 - copy raw data here'!F8</f>
-        <v>0.94583763538108701</v>
-      </c>
-      <c r="D9" s="44">
+        <v>1.2283358760619401</v>
+      </c>
+      <c r="D9" s="90">
         <f>'Table 1 - copy raw data here'!G8</f>
-        <v>0.79808015401854604</v>
+        <v>0.86337590372881601</v>
       </c>
       <c r="E9" s="29">
         <f>'Table 1 - copy raw data here'!B8/100</f>
-        <v>-7.0999999999999994E-2</v>
-      </c>
-      <c r="F9" s="45">
+        <v>0.48700000000000004</v>
+      </c>
+      <c r="F9" s="87">
         <f>'Table 1 - copy raw data here'!C8/100</f>
-        <v>0.01</v>
-      </c>
-      <c r="G9" s="42">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="G9" s="86">
         <f>'Table 1 - copy raw data here'!D8/100</f>
-        <v>-3.3000000000000002E-2</v>
+        <v>0.33899999999999997</v>
       </c>
       <c r="H9" s="27">
         <f>'Table 1 - copy raw data here'!K8</f>
-        <v>0.28229740201522902</v>
+        <v>0.441917209407449</v>
       </c>
       <c r="I9" s="28">
         <f>'Table 1 - copy raw data here'!L8</f>
-        <v>0.28618404634260602</v>
-      </c>
-      <c r="J9" s="93">
+        <v>0.48907248286788402</v>
+      </c>
+      <c r="J9" s="28">
         <f>'Table 1 - copy raw data here'!M8</f>
-        <v>0.34340558384439301</v>
+        <v>0.37111742539425402</v>
       </c>
       <c r="K9" s="27">
         <f>'Table 1 - copy raw data here'!H8</f>
-        <v>0.93563642400835201</v>
+        <v>0.96972039389537301</v>
       </c>
       <c r="L9" s="28">
         <f>'Table 1 - copy raw data here'!I8</f>
-        <v>0.91094405569218295</v>
-      </c>
-      <c r="M9" s="40">
+        <v>0.90988591409012798</v>
+      </c>
+      <c r="M9" s="85">
         <f>'Table 1 - copy raw data here'!J8</f>
-        <v>0.90558260577088101</v>
+        <v>0.69401816999657095</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="34">
+      <c r="B10" s="32">
         <f>AVERAGE(B3:B9)</f>
-        <v>1.2670502327393487</v>
-      </c>
-      <c r="C10" s="47">
+        <v>1.6453730527578301</v>
+      </c>
+      <c r="C10" s="83">
         <f t="shared" ref="C10:M10" si="0">AVERAGE(C3:C9)</f>
-        <v>1.1454691983229759</v>
-      </c>
-      <c r="D10" s="32">
+        <v>1.4564653408714938</v>
+      </c>
+      <c r="D10" s="37">
         <f t="shared" si="0"/>
-        <v>1.2020338403521376</v>
-      </c>
-      <c r="E10" s="37">
+        <v>1.4390239191340108</v>
+      </c>
+      <c r="E10" s="35">
         <f t="shared" si="0"/>
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="F10" s="48">
+        <v>0.79485714285714282</v>
+      </c>
+      <c r="F10" s="84">
         <f t="shared" si="0"/>
-        <v>0.12142857142857143</v>
-      </c>
-      <c r="G10" s="33">
+        <v>0.71128571428571441</v>
+      </c>
+      <c r="G10" s="38">
         <f t="shared" si="0"/>
-        <v>0.21199999999999999</v>
-      </c>
-      <c r="H10" s="34">
+        <v>0.64900000000000013</v>
+      </c>
+      <c r="H10" s="32">
         <f t="shared" si="0"/>
-        <v>0.26706607624344858</v>
-      </c>
-      <c r="I10" s="47">
+        <v>0.42424791180768728</v>
+      </c>
+      <c r="I10" s="37">
         <f t="shared" si="0"/>
-        <v>0.27872490022939156</v>
-      </c>
-      <c r="J10" s="47">
+        <v>0.46406106348177428</v>
+      </c>
+      <c r="J10" s="83">
         <f t="shared" si="0"/>
-        <v>0.28111091116228798</v>
-      </c>
-      <c r="K10" s="49">
+        <v>0.32491716582232144</v>
+      </c>
+      <c r="K10" s="39">
         <f t="shared" si="0"/>
-        <v>0.93459471810237704</v>
-      </c>
-      <c r="L10" s="35">
+        <v>0.93500486668490457</v>
+      </c>
+      <c r="L10" s="33">
         <f t="shared" si="0"/>
-        <v>0.88891016746263973</v>
-      </c>
-      <c r="M10" s="36">
+        <v>0.87739683236734556</v>
+      </c>
+      <c r="M10" s="34">
         <f t="shared" si="0"/>
-        <v>0.84456716566968226</v>
+        <v>0.60587569612727754</v>
       </c>
     </row>
   </sheetData>
@@ -1879,13 +1885,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>7.9843275851626205E-2</v>
+        <v>9.2940388488922707E-2</v>
       </c>
       <c r="D2">
-        <v>0.96608893313863498</v>
+        <v>0.95392405937265901</v>
       </c>
       <c r="E2">
-        <v>1.01089537141909</v>
+        <v>1.01020632147573</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1896,13 +1902,13 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.33006284778181</v>
+        <v>0.340981905337637</v>
       </c>
       <c r="D3">
-        <v>0.50274477265071504</v>
+        <v>0.46154690097069101</v>
       </c>
       <c r="E3">
-        <v>0.61605225503431105</v>
+        <v>0.564953094661791</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1913,13 +1919,13 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0.11268165096900799</v>
+        <v>0.16927279982131699</v>
       </c>
       <c r="D4">
-        <v>0.92275076563106995</v>
+        <v>0.85119026125060704</v>
       </c>
       <c r="E4">
-        <v>1.0010578728958399</v>
+        <v>0.96916176826951494</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1930,13 +1936,13 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0.24973661778678599</v>
+        <v>0.18379400931050499</v>
       </c>
       <c r="D5">
-        <v>0.65056524434603202</v>
+        <v>0.78498217394466796</v>
       </c>
       <c r="E5">
-        <v>0.80785136393214096</v>
+        <v>0.84537688322844495</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1947,13 +1953,13 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>9.9349474711792798E-2</v>
+        <v>0.122234561255987</v>
       </c>
       <c r="D6">
-        <v>0.930632854423041</v>
+        <v>0.90151033916294798</v>
       </c>
       <c r="E6">
-        <v>1.0049985912446799</v>
+        <v>0.96072006766502605</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1964,13 +1970,13 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>1.9286508155455399E-2</v>
+        <v>0.10041277669412101</v>
       </c>
       <c r="D7">
-        <v>0.99793938228183798</v>
+        <v>0.94946093017919098</v>
       </c>
       <c r="E7">
-        <v>1.0098242848396499</v>
+        <v>1.0199820836896401</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1981,13 +1987,13 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0.14938623912125501</v>
+        <v>0.13208980592191499</v>
       </c>
       <c r="D8">
-        <v>0.88398014198517305</v>
+        <v>0.89369366323562704</v>
       </c>
       <c r="E8">
-        <v>0.93459274167575601</v>
+        <v>0.96124285380409002</v>
       </c>
     </row>
   </sheetData>
@@ -1999,8 +2005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926FA25B-0675-4415-9EAE-A1DBC10ABC93}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2010,7 +2016,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="45" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="30" t="s">
@@ -2025,154 +2031,154 @@
       <c r="E1" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="54"/>
+      <c r="F1" s="44"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="57">
+      <c r="B2" s="47">
         <f>'Table S1 copy raw data'!C2</f>
-        <v>7.9843275851626205E-2</v>
-      </c>
-      <c r="C2" s="58">
+        <v>9.2940388488922707E-2</v>
+      </c>
+      <c r="C2" s="48">
         <f>'Table S1 copy raw data'!B2</f>
         <v>0</v>
       </c>
-      <c r="D2" s="59">
+      <c r="D2" s="49">
         <f>'Table S1 copy raw data'!E2</f>
-        <v>1.01089537141909</v>
-      </c>
-      <c r="E2" s="60">
+        <v>1.01020632147573</v>
+      </c>
+      <c r="E2" s="50">
         <f>'Table S1 copy raw data'!D2</f>
-        <v>0.96608893313863498</v>
+        <v>0.95392405937265901</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="57">
+      <c r="B3" s="47">
         <f>'Table S1 copy raw data'!C3</f>
-        <v>0.33006284778181</v>
-      </c>
-      <c r="C3" s="58">
+        <v>0.340981905337637</v>
+      </c>
+      <c r="C3" s="48">
         <f>'Table S1 copy raw data'!B3</f>
         <v>0</v>
       </c>
-      <c r="D3" s="59">
+      <c r="D3" s="49">
         <f>'Table S1 copy raw data'!E3</f>
-        <v>0.61605225503431105</v>
-      </c>
-      <c r="E3" s="60">
+        <v>0.564953094661791</v>
+      </c>
+      <c r="E3" s="50">
         <f>'Table S1 copy raw data'!D3</f>
-        <v>0.50274477265071504</v>
+        <v>0.46154690097069101</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="57">
+      <c r="B4" s="47">
         <f>'Table S1 copy raw data'!C4</f>
-        <v>0.11268165096900799</v>
-      </c>
-      <c r="C4" s="58">
+        <v>0.16927279982131699</v>
+      </c>
+      <c r="C4" s="48">
         <f>'Table S1 copy raw data'!B4</f>
         <v>0</v>
       </c>
-      <c r="D4" s="59">
+      <c r="D4" s="49">
         <f>'Table S1 copy raw data'!E4</f>
-        <v>1.0010578728958399</v>
-      </c>
-      <c r="E4" s="60">
+        <v>0.96916176826951494</v>
+      </c>
+      <c r="E4" s="50">
         <f>'Table S1 copy raw data'!D4</f>
-        <v>0.92275076563106995</v>
+        <v>0.85119026125060704</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="57">
+      <c r="B5" s="47">
         <f>'Table S1 copy raw data'!C5</f>
-        <v>0.24973661778678599</v>
-      </c>
-      <c r="C5" s="58">
+        <v>0.18379400931050499</v>
+      </c>
+      <c r="C5" s="48">
         <f>'Table S1 copy raw data'!B5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="59">
+      <c r="D5" s="49">
         <f>'Table S1 copy raw data'!E5</f>
-        <v>0.80785136393214096</v>
-      </c>
-      <c r="E5" s="60">
+        <v>0.84537688322844495</v>
+      </c>
+      <c r="E5" s="50">
         <f>'Table S1 copy raw data'!D5</f>
-        <v>0.65056524434603202</v>
+        <v>0.78498217394466796</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="57">
+      <c r="B6" s="47">
         <f>'Table S1 copy raw data'!C6</f>
-        <v>9.9349474711792798E-2</v>
-      </c>
-      <c r="C6" s="58">
+        <v>0.122234561255987</v>
+      </c>
+      <c r="C6" s="48">
         <f>'Table S1 copy raw data'!B6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="59">
+      <c r="D6" s="49">
         <f>'Table S1 copy raw data'!E6</f>
-        <v>1.0049985912446799</v>
-      </c>
-      <c r="E6" s="60">
+        <v>0.96072006766502605</v>
+      </c>
+      <c r="E6" s="50">
         <f>'Table S1 copy raw data'!D6</f>
-        <v>0.930632854423041</v>
+        <v>0.90151033916294798</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="57">
+      <c r="B7" s="47">
         <f>'Table S1 copy raw data'!C7</f>
-        <v>1.9286508155455399E-2</v>
-      </c>
-      <c r="C7" s="58">
+        <v>0.10041277669412101</v>
+      </c>
+      <c r="C7" s="48">
         <f>'Table S1 copy raw data'!B7</f>
         <v>0</v>
       </c>
-      <c r="D7" s="59">
+      <c r="D7" s="49">
         <f>'Table S1 copy raw data'!E7</f>
-        <v>1.0098242848396499</v>
-      </c>
-      <c r="E7" s="60">
+        <v>1.0199820836896401</v>
+      </c>
+      <c r="E7" s="50">
         <f>'Table S1 copy raw data'!D7</f>
-        <v>0.99793938228183798</v>
+        <v>0.94946093017919098</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="57">
+      <c r="B8" s="47">
         <f>'Table S1 copy raw data'!C8</f>
-        <v>0.14938623912125501</v>
-      </c>
-      <c r="C8" s="58">
+        <v>0.13208980592191499</v>
+      </c>
+      <c r="C8" s="48">
         <f>'Table S1 copy raw data'!B8</f>
         <v>0</v>
       </c>
-      <c r="D8" s="59">
+      <c r="D8" s="49">
         <f>'Table S1 copy raw data'!E8</f>
-        <v>0.93459274167575601</v>
-      </c>
-      <c r="E8" s="60">
+        <v>0.96124285380409002</v>
+      </c>
+      <c r="E8" s="50">
         <f>'Table S1 copy raw data'!D8</f>
-        <v>0.88398014198517305</v>
+        <v>0.89369366323562704</v>
       </c>
     </row>
   </sheetData>
@@ -2185,7 +2191,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+      <selection sqref="A1:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2215,16 +2221,16 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>-2.1</v>
+        <v>14.7</v>
       </c>
       <c r="C2">
-        <v>158.83670079153501</v>
+        <v>145.63510790120901</v>
       </c>
       <c r="D2">
-        <v>0.14925647947771201</v>
+        <v>0.16558424807591199</v>
       </c>
       <c r="E2">
-        <v>0.36435489412809002</v>
+        <v>0.47014517086380903</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -2235,16 +2241,16 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>36.200000000000003</v>
+        <v>53</v>
       </c>
       <c r="C3">
-        <v>208.573091116265</v>
+        <v>222.54464309897301</v>
       </c>
       <c r="D3">
-        <v>0.15191706857592699</v>
+        <v>0.159415768085021</v>
       </c>
       <c r="E3">
-        <v>0.27763651089607999</v>
+        <v>0.32618257824870001</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -2255,16 +2261,16 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="C4">
-        <v>154.24716734549</v>
+        <v>142.75054632827599</v>
       </c>
       <c r="D4">
-        <v>0.17553976672256899</v>
+        <v>0.199570171231125</v>
       </c>
       <c r="E4">
-        <v>0.39957897070387199</v>
+        <v>0.52362784643197202</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -2275,16 +2281,16 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>-44.3</v>
+        <v>-29.5</v>
       </c>
       <c r="C5">
-        <v>193.51904132870399</v>
+        <v>157.47284111953701</v>
       </c>
       <c r="D5">
-        <v>0.20022441309066299</v>
+        <v>0.21098245367756199</v>
       </c>
       <c r="E5">
-        <v>0.46786228323747497</v>
+        <v>0.54043995425047398</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -2295,16 +2301,16 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>-17.600000000000001</v>
+        <v>-0.9</v>
       </c>
       <c r="C6">
-        <v>160.428672913577</v>
+        <v>139.66097462927701</v>
       </c>
       <c r="D6">
-        <v>0.110529415139272</v>
+        <v>0.113886370151475</v>
       </c>
       <c r="E6">
-        <v>0.36863747561622201</v>
+        <v>0.46981089329105102</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -2315,16 +2321,16 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>55.5</v>
+        <v>72.400000000000006</v>
       </c>
       <c r="C7">
-        <v>237.034461967254</v>
+        <v>279.56460329244601</v>
       </c>
       <c r="D7">
-        <v>6.5466048596065501E-2</v>
+        <v>6.15220402826121E-2</v>
       </c>
       <c r="E7">
-        <v>0.234391905366129</v>
+        <v>0.27856920003521501</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -2335,16 +2341,16 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>0.2</v>
+        <v>16.7</v>
       </c>
       <c r="C8">
-        <v>157.78847803505801</v>
+        <v>144.341525553043</v>
       </c>
       <c r="D8">
-        <v>0.21200295801792801</v>
+        <v>0.24086493137075801</v>
       </c>
       <c r="E8">
-        <v>0.39201007916068698</v>
+        <v>0.48963860411815502</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
@@ -2355,16 +2361,16 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>-3.7</v>
+        <v>12.2</v>
       </c>
       <c r="C9">
-        <v>86.676236646068105</v>
+        <v>98.874492262887699</v>
       </c>
       <c r="D9">
-        <v>0.40106600584448998</v>
+        <v>0.35674008376359601</v>
       </c>
       <c r="E9">
-        <v>0.86164404835919906</v>
+        <v>0.87094991566539404</v>
       </c>
       <c r="F9" t="s">
         <v>34</v>
@@ -2375,16 +2381,16 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>33.6</v>
+        <v>49.6</v>
       </c>
       <c r="C10">
-        <v>140.09986888491301</v>
+        <v>190.131853581462</v>
       </c>
       <c r="D10">
-        <v>0.44557669366817398</v>
+        <v>0.424228374684327</v>
       </c>
       <c r="E10">
-        <v>0.69282968059709704</v>
+        <v>0.72327523984244202</v>
       </c>
       <c r="F10" t="s">
         <v>34</v>
@@ -2395,16 +2401,16 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>-1.5</v>
+        <v>14.4</v>
       </c>
       <c r="C11">
-        <v>84.810872632814394</v>
+        <v>99.603747299688393</v>
       </c>
       <c r="D11">
-        <v>0.43513330302387698</v>
+        <v>0.39908717943623601</v>
       </c>
       <c r="E11">
-        <v>0.90921286467112905</v>
+        <v>0.94534026810471095</v>
       </c>
       <c r="F11" t="s">
         <v>34</v>
@@ -2415,16 +2421,16 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>-45.3</v>
+        <v>-31.3</v>
       </c>
       <c r="C12">
-        <v>168.690255571888</v>
+        <v>123.92817748618199</v>
       </c>
       <c r="D12">
-        <v>0.44003666382415402</v>
+        <v>0.373040091440559</v>
       </c>
       <c r="E12">
-        <v>0.97362933474074598</v>
+        <v>0.89084759779255096</v>
       </c>
       <c r="F12" t="s">
         <v>34</v>
@@ -2435,16 +2441,16 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>-19.2</v>
+        <v>-3.3</v>
       </c>
       <c r="C13">
-        <v>99.039687311519501</v>
+        <v>101.649558801711</v>
       </c>
       <c r="D13">
-        <v>0.214710871542101</v>
+        <v>0.169274581569167</v>
       </c>
       <c r="E13">
-        <v>0.67864264295438703</v>
+        <v>0.649411350496922</v>
       </c>
       <c r="F13" t="s">
         <v>34</v>
@@ -2455,16 +2461,16 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>52.2</v>
+        <v>68.2</v>
       </c>
       <c r="C14">
-        <v>204.40437071949901</v>
+        <v>258.99252047032201</v>
       </c>
       <c r="D14">
-        <v>0.16307516295921401</v>
+        <v>0.12538173855728399</v>
       </c>
       <c r="E14">
-        <v>0.54285206096132699</v>
+        <v>0.51385254197861896</v>
       </c>
       <c r="F14" t="s">
         <v>34</v>
@@ -2475,16 +2481,16 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>-1.3</v>
+        <v>14.4</v>
       </c>
       <c r="C15">
-        <v>61.825709179357297</v>
+        <v>89.848002117268393</v>
       </c>
       <c r="D15">
-        <v>0.60633357551690403</v>
+        <v>0.56024285483421699</v>
       </c>
       <c r="E15">
-        <v>1.0380621339618601</v>
+        <v>1.0560030090570101</v>
       </c>
       <c r="F15" t="s">
         <v>34</v>
@@ -2500,7 +2506,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2517,50 +2523,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="62"/>
-      <c r="B1" s="63" t="s">
+      <c r="A1" s="51"/>
+      <c r="B1" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="63" t="s">
+      <c r="C1" s="82"/>
+      <c r="D1" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="64"/>
-      <c r="F1" s="63" t="s">
+      <c r="E1" s="82"/>
+      <c r="F1" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="64"/>
-      <c r="H1" s="63" t="s">
+      <c r="G1" s="82"/>
+      <c r="H1" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="64"/>
+      <c r="I1" s="82"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="C2" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="68" t="s">
+      <c r="I2" s="55" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2568,296 +2574,296 @@
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="81">
+      <c r="B3" s="68">
         <f>'Table 2 - copy raw data here'!C2</f>
-        <v>158.83670079153501</v>
-      </c>
-      <c r="C3" s="82">
+        <v>145.63510790120901</v>
+      </c>
+      <c r="C3" s="69">
         <f>'Table 2 - copy raw data here'!C9</f>
-        <v>86.676236646068105</v>
-      </c>
-      <c r="D3" s="83">
+        <v>98.874492262887699</v>
+      </c>
+      <c r="D3" s="70">
         <f>'Table 2 - copy raw data here'!B2</f>
-        <v>-2.1</v>
-      </c>
-      <c r="E3" s="84">
+        <v>14.7</v>
+      </c>
+      <c r="E3" s="71">
         <f>'Table 2 - copy raw data here'!B9</f>
-        <v>-3.7</v>
-      </c>
-      <c r="F3" s="85">
+        <v>12.2</v>
+      </c>
+      <c r="F3" s="72">
         <f>'Table 2 - copy raw data here'!E2</f>
-        <v>0.36435489412809002</v>
-      </c>
-      <c r="G3" s="86">
+        <v>0.47014517086380903</v>
+      </c>
+      <c r="G3" s="73">
         <f>'Table 2 - copy raw data here'!E9</f>
-        <v>0.86164404835919906</v>
-      </c>
-      <c r="H3" s="85">
+        <v>0.87094991566539404</v>
+      </c>
+      <c r="H3" s="72">
         <f>'Table 2 - copy raw data here'!D2</f>
-        <v>0.14925647947771201</v>
-      </c>
-      <c r="I3" s="86">
+        <v>0.16558424807591199</v>
+      </c>
+      <c r="I3" s="73">
         <f>'Table 2 - copy raw data here'!D9</f>
-        <v>0.40106600584448998</v>
+        <v>0.35674008376359601</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="69">
+      <c r="B4" s="56">
         <f>'Table 2 - copy raw data here'!C3</f>
-        <v>208.573091116265</v>
-      </c>
-      <c r="C4" s="70">
+        <v>222.54464309897301</v>
+      </c>
+      <c r="C4" s="57">
         <f>'Table 2 - copy raw data here'!C10</f>
-        <v>140.09986888491301</v>
-      </c>
-      <c r="D4" s="71">
+        <v>190.131853581462</v>
+      </c>
+      <c r="D4" s="58">
         <f>'Table 2 - copy raw data here'!B3</f>
-        <v>36.200000000000003</v>
-      </c>
-      <c r="E4" s="72">
+        <v>53</v>
+      </c>
+      <c r="E4" s="59">
         <f>'Table 2 - copy raw data here'!B10</f>
-        <v>33.6</v>
-      </c>
-      <c r="F4" s="73">
+        <v>49.6</v>
+      </c>
+      <c r="F4" s="60">
         <f>'Table 2 - copy raw data here'!E3</f>
-        <v>0.27763651089607999</v>
-      </c>
-      <c r="G4" s="74">
+        <v>0.32618257824870001</v>
+      </c>
+      <c r="G4" s="61">
         <f>'Table 2 - copy raw data here'!E10</f>
-        <v>0.69282968059709704</v>
-      </c>
-      <c r="H4" s="73">
+        <v>0.72327523984244202</v>
+      </c>
+      <c r="H4" s="60">
         <f>'Table 2 - copy raw data here'!D3</f>
-        <v>0.15191706857592699</v>
-      </c>
-      <c r="I4" s="74">
+        <v>0.159415768085021</v>
+      </c>
+      <c r="I4" s="61">
         <f>'Table 2 - copy raw data here'!D10</f>
-        <v>0.44557669366817398</v>
+        <v>0.424228374684327</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="81">
+      <c r="B5" s="68">
         <f>'Table 2 - copy raw data here'!C4</f>
-        <v>154.24716734549</v>
-      </c>
-      <c r="C5" s="82">
+        <v>142.75054632827599</v>
+      </c>
+      <c r="C5" s="69">
         <f>'Table 2 - copy raw data here'!C11</f>
-        <v>84.810872632814394</v>
-      </c>
-      <c r="D5" s="83">
+        <v>99.603747299688393</v>
+      </c>
+      <c r="D5" s="70">
         <f>'Table 2 - copy raw data here'!B4</f>
-        <v>0.1</v>
-      </c>
-      <c r="E5" s="84">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E5" s="71">
         <f>'Table 2 - copy raw data here'!B11</f>
-        <v>-1.5</v>
-      </c>
-      <c r="F5" s="85">
+        <v>14.4</v>
+      </c>
+      <c r="F5" s="72">
         <f>'Table 2 - copy raw data here'!E4</f>
-        <v>0.39957897070387199</v>
-      </c>
-      <c r="G5" s="86">
+        <v>0.52362784643197202</v>
+      </c>
+      <c r="G5" s="73">
         <f>'Table 2 - copy raw data here'!E11</f>
-        <v>0.90921286467112905</v>
-      </c>
-      <c r="H5" s="85">
+        <v>0.94534026810471095</v>
+      </c>
+      <c r="H5" s="72">
         <f>'Table 2 - copy raw data here'!D4</f>
-        <v>0.17553976672256899</v>
-      </c>
-      <c r="I5" s="86">
+        <v>0.199570171231125</v>
+      </c>
+      <c r="I5" s="73">
         <f>'Table 2 - copy raw data here'!D11</f>
-        <v>0.43513330302387698</v>
+        <v>0.39908717943623601</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="69">
+      <c r="B6" s="56">
         <f>'Table 2 - copy raw data here'!C5</f>
-        <v>193.51904132870399</v>
-      </c>
-      <c r="C6" s="70">
+        <v>157.47284111953701</v>
+      </c>
+      <c r="C6" s="57">
         <f>'Table 2 - copy raw data here'!C12</f>
-        <v>168.690255571888</v>
-      </c>
-      <c r="D6" s="71">
+        <v>123.92817748618199</v>
+      </c>
+      <c r="D6" s="58">
         <f>'Table 2 - copy raw data here'!B5</f>
-        <v>-44.3</v>
-      </c>
-      <c r="E6" s="72">
+        <v>-29.5</v>
+      </c>
+      <c r="E6" s="59">
         <f>'Table 2 - copy raw data here'!B12</f>
-        <v>-45.3</v>
-      </c>
-      <c r="F6" s="73">
+        <v>-31.3</v>
+      </c>
+      <c r="F6" s="60">
         <f>'Table 2 - copy raw data here'!E5</f>
-        <v>0.46786228323747497</v>
-      </c>
-      <c r="G6" s="74">
+        <v>0.54043995425047398</v>
+      </c>
+      <c r="G6" s="61">
         <f>'Table 2 - copy raw data here'!E12</f>
-        <v>0.97362933474074598</v>
-      </c>
-      <c r="H6" s="73">
+        <v>0.89084759779255096</v>
+      </c>
+      <c r="H6" s="60">
         <f>'Table 2 - copy raw data here'!D5</f>
-        <v>0.20022441309066299</v>
-      </c>
-      <c r="I6" s="74">
+        <v>0.21098245367756199</v>
+      </c>
+      <c r="I6" s="61">
         <f>'Table 2 - copy raw data here'!D12</f>
-        <v>0.44003666382415402</v>
+        <v>0.373040091440559</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="81">
+      <c r="B7" s="68">
         <f>'Table 2 - copy raw data here'!C6</f>
-        <v>160.428672913577</v>
-      </c>
-      <c r="C7" s="82">
+        <v>139.66097462927701</v>
+      </c>
+      <c r="C7" s="69">
         <f>'Table 2 - copy raw data here'!C13</f>
-        <v>99.039687311519501</v>
-      </c>
-      <c r="D7" s="83">
+        <v>101.649558801711</v>
+      </c>
+      <c r="D7" s="70">
         <f>'Table 2 - copy raw data here'!B6</f>
-        <v>-17.600000000000001</v>
-      </c>
-      <c r="E7" s="84">
+        <v>-0.9</v>
+      </c>
+      <c r="E7" s="71">
         <f>'Table 2 - copy raw data here'!B13</f>
-        <v>-19.2</v>
-      </c>
-      <c r="F7" s="85">
+        <v>-3.3</v>
+      </c>
+      <c r="F7" s="72">
         <f>'Table 2 - copy raw data here'!E6</f>
-        <v>0.36863747561622201</v>
-      </c>
-      <c r="G7" s="86">
+        <v>0.46981089329105102</v>
+      </c>
+      <c r="G7" s="73">
         <f>'Table 2 - copy raw data here'!E13</f>
-        <v>0.67864264295438703</v>
-      </c>
-      <c r="H7" s="85">
+        <v>0.649411350496922</v>
+      </c>
+      <c r="H7" s="72">
         <f>'Table 2 - copy raw data here'!D6</f>
-        <v>0.110529415139272</v>
-      </c>
-      <c r="I7" s="86">
+        <v>0.113886370151475</v>
+      </c>
+      <c r="I7" s="73">
         <f>'Table 2 - copy raw data here'!D13</f>
-        <v>0.214710871542101</v>
+        <v>0.169274581569167</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="69">
+      <c r="B8" s="56">
         <f>'Table 2 - copy raw data here'!C7</f>
-        <v>237.034461967254</v>
-      </c>
-      <c r="C8" s="70">
+        <v>279.56460329244601</v>
+      </c>
+      <c r="C8" s="57">
         <f>'Table 2 - copy raw data here'!C14</f>
-        <v>204.40437071949901</v>
-      </c>
-      <c r="D8" s="71">
+        <v>258.99252047032201</v>
+      </c>
+      <c r="D8" s="58">
         <f>'Table 2 - copy raw data here'!B7</f>
-        <v>55.5</v>
-      </c>
-      <c r="E8" s="72">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="E8" s="59">
         <f>'Table 2 - copy raw data here'!B14</f>
-        <v>52.2</v>
-      </c>
-      <c r="F8" s="73">
+        <v>68.2</v>
+      </c>
+      <c r="F8" s="60">
         <f>'Table 2 - copy raw data here'!E7</f>
-        <v>0.234391905366129</v>
-      </c>
-      <c r="G8" s="74">
+        <v>0.27856920003521501</v>
+      </c>
+      <c r="G8" s="61">
         <f>'Table 2 - copy raw data here'!E14</f>
-        <v>0.54285206096132699</v>
-      </c>
-      <c r="H8" s="73">
+        <v>0.51385254197861896</v>
+      </c>
+      <c r="H8" s="60">
         <f>'Table 2 - copy raw data here'!D7</f>
-        <v>6.5466048596065501E-2</v>
-      </c>
-      <c r="I8" s="74">
+        <v>6.15220402826121E-2</v>
+      </c>
+      <c r="I8" s="61">
         <f>'Table 2 - copy raw data here'!D14</f>
-        <v>0.16307516295921401</v>
+        <v>0.12538173855728399</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="87">
+      <c r="B9" s="74">
         <f>'Table 2 - copy raw data here'!C8</f>
-        <v>157.78847803505801</v>
-      </c>
-      <c r="C9" s="88">
+        <v>144.341525553043</v>
+      </c>
+      <c r="C9" s="75">
         <f>'Table 2 - copy raw data here'!C15</f>
-        <v>61.825709179357297</v>
-      </c>
-      <c r="D9" s="89">
+        <v>89.848002117268393</v>
+      </c>
+      <c r="D9" s="76">
         <f>'Table 2 - copy raw data here'!B8</f>
-        <v>0.2</v>
-      </c>
-      <c r="E9" s="90">
+        <v>16.7</v>
+      </c>
+      <c r="E9" s="77">
         <f>'Table 2 - copy raw data here'!B15</f>
-        <v>-1.3</v>
-      </c>
-      <c r="F9" s="91">
+        <v>14.4</v>
+      </c>
+      <c r="F9" s="78">
         <f>'Table 2 - copy raw data here'!E8</f>
-        <v>0.39201007916068698</v>
-      </c>
-      <c r="G9" s="92">
+        <v>0.48963860411815502</v>
+      </c>
+      <c r="G9" s="79">
         <f>'Table 2 - copy raw data here'!E15</f>
-        <v>1.0380621339618601</v>
-      </c>
-      <c r="H9" s="91">
+        <v>1.0560030090570101</v>
+      </c>
+      <c r="H9" s="78">
         <f>'Table 2 - copy raw data here'!D8</f>
-        <v>0.21200295801792801</v>
-      </c>
-      <c r="I9" s="92">
+        <v>0.24086493137075801</v>
+      </c>
+      <c r="I9" s="79">
         <f>'Table 2 - copy raw data here'!D15</f>
-        <v>0.60633357551690403</v>
+        <v>0.56024285483421699</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="75">
+      <c r="B10" s="62">
         <f>AVERAGE(B3:B9)</f>
-        <v>181.48965907112614</v>
-      </c>
-      <c r="C10" s="76">
+        <v>175.99574884610871</v>
+      </c>
+      <c r="C10" s="63">
         <f t="shared" ref="C10:I10" si="0">AVERAGE(C3:C9)</f>
-        <v>120.79242870657991</v>
-      </c>
-      <c r="D10" s="77">
+        <v>137.57547885993162</v>
+      </c>
+      <c r="D10" s="64">
         <f t="shared" si="0"/>
-        <v>4.0000000000000009</v>
-      </c>
-      <c r="E10" s="78">
+        <v>20.471428571428568</v>
+      </c>
+      <c r="E10" s="65">
         <f t="shared" si="0"/>
-        <v>2.1142857142857152</v>
-      </c>
-      <c r="F10" s="79">
+        <v>17.742857142857144</v>
+      </c>
+      <c r="F10" s="66">
         <f t="shared" si="0"/>
-        <v>0.35778173130122209</v>
-      </c>
-      <c r="G10" s="80">
+        <v>0.44263060674848231</v>
+      </c>
+      <c r="G10" s="67">
         <f t="shared" si="0"/>
-        <v>0.81383896660653499</v>
-      </c>
-      <c r="H10" s="79">
+        <v>0.80709713184823573</v>
+      </c>
+      <c r="H10" s="66">
         <f t="shared" si="0"/>
-        <v>0.1521337356600195</v>
-      </c>
-      <c r="I10" s="80">
+        <v>0.16454656898206643</v>
+      </c>
+      <c r="I10" s="67">
         <f t="shared" si="0"/>
-        <v>0.38656175376841634</v>
+        <v>0.34399927204076947</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to initial submission for Ag Water Management
</commit_message>
<xml_diff>
--- a/figures+tables/Compare_OpenET-WIMAS_LEMA_allts_FitStats_Formatted.xlsx
+++ b/figures+tables/Compare_OpenET-WIMAS_LEMA_allts_FitStats_Formatted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s947z036\WorkGits\SD-6_MapWaterConservation\figures+tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A9C289-1D70-4036-B303-BAB193253A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FAE20D-50F3-423B-803C-4E82340EDC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 - copy raw data here" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Table S1 Precip corrected table" sheetId="4" r:id="rId4"/>
     <sheet name="Table 2 - copy raw data here" sheetId="5" r:id="rId5"/>
     <sheet name="Table 2 formatted" sheetId="6" r:id="rId6"/>
+    <sheet name="Table S2 - copy raw data here" sheetId="8" r:id="rId7"/>
+    <sheet name="Table S2 formatted" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="49">
   <si>
     <t>Algorithm</t>
   </si>
@@ -95,12 +97,6 @@
     <t>Annual</t>
   </si>
   <si>
-    <t>Growing Season</t>
-  </si>
-  <si>
-    <t>Water Year</t>
-  </si>
-  <si>
     <t>Bias [%]</t>
   </si>
   <si>
@@ -135,6 +131,64 @@
   </si>
   <si>
     <t>MAE_1e7m3_Water Year</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Best in column</t>
+  </si>
+  <si>
+    <t>Best for metric</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Best average across algorithms</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Bias_prc</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>MAE_mm</t>
+  </si>
+  <si>
+    <t>MAE [mm]</t>
+  </si>
+  <si>
+    <t>Multi-Year</t>
+  </si>
+  <si>
+    <t>MAE_1e7m3</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
   </si>
   <si>
     <r>
@@ -144,22 +198,20 @@
       <rPr>
         <b/>
         <vertAlign val="superscript"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>7</t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> m</t>
     </r>
@@ -167,87 +219,32 @@
       <rPr>
         <b/>
         <vertAlign val="superscript"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>3</t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>]</t>
     </r>
   </si>
   <si>
-    <r>
-      <t>R</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Best in column</t>
-  </si>
-  <si>
-    <t>Best for metric</t>
-  </si>
-  <si>
-    <t>Legend</t>
-  </si>
-  <si>
-    <t>Best average across algorithms</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Bias_prc</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>slope</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>MAE_mm</t>
-  </si>
-  <si>
-    <t>MAE [mm]</t>
-  </si>
-  <si>
-    <t>Multi-Year</t>
-  </si>
-  <si>
-    <t>MAE_1e7m3</t>
-  </si>
-  <si>
-    <t>Calendar Year</t>
+    <t>C.Y.</t>
+  </si>
+  <si>
+    <t>G.S.</t>
+  </si>
+  <si>
+    <t>W.Y.</t>
   </si>
 </sst>
 </file>
@@ -274,31 +271,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <vertAlign val="superscript"/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -314,12 +287,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <i/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -354,7 +347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -494,206 +487,262 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1001,13 +1050,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -1325,515 +1374,512 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="6.28515625" customWidth="1"/>
     <col min="14" max="14" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="80" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80" t="s">
+    <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="18"/>
+      <c r="B1" s="90" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-    </row>
-    <row r="2" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="7">
+      <c r="B3" s="55">
         <f>'Table 1 - copy raw data here'!E2</f>
         <v>1.3264925760619399</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="56">
         <f>'Table 1 - copy raw data here'!F2</f>
         <v>0.94977537606193996</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="57">
         <f>'Table 1 - copy raw data here'!G2</f>
         <v>1.1936025751473101</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="58">
         <f>'Table 1 - copy raw data here'!B2/100</f>
         <v>0.65400000000000003</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="59">
         <f>'Table 1 - copy raw data here'!C2/100</f>
         <v>0.46799999999999997</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="60">
         <f>'Table 1 - copy raw data here'!D2/100</f>
         <v>0.50600000000000001</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="55">
         <f>'Table 1 - copy raw data here'!K2</f>
         <v>0.40690748489495798</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="56">
         <f>'Table 1 - copy raw data here'!L2</f>
         <v>0.43274806461895099</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="56">
         <f>'Table 1 - copy raw data here'!M2</f>
         <v>0.22662206988995201</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="55">
         <f>'Table 1 - copy raw data here'!H2</f>
         <v>0.70722325678104503</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="56">
         <f>'Table 1 - copy raw data here'!I2</f>
         <v>0.69082503808143803</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="57">
         <f>'Table 1 - copy raw data here'!J2</f>
         <v>0.31761842437134202</v>
       </c>
-      <c r="N3" s="43" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="14">
+      <c r="N3" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="61">
         <f>'Table 1 - copy raw data here'!E3</f>
         <v>2.2049506480619399</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="23">
         <f>'Table 1 - copy raw data here'!F3</f>
         <v>2.00024414806194</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="24">
         <f>'Table 1 - copy raw data here'!G3</f>
         <v>1.85773088406194</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="62">
         <f>'Table 1 - copy raw data here'!B3/100</f>
         <v>1.0859999999999999</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="63">
         <f>'Table 1 - copy raw data here'!C3/100</f>
         <v>0.98499999999999999</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="64">
         <f>'Table 1 - copy raw data here'!D3/100</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="61">
         <f>'Table 1 - copy raw data here'!K3</f>
         <v>0.377574803193928</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="23">
         <f>'Table 1 - copy raw data here'!L3</f>
         <v>0.38775196783792598</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="23">
         <f>'Table 1 - copy raw data here'!M3</f>
         <v>0.28503364673370002</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="61">
         <f>'Table 1 - copy raw data here'!H3</f>
         <v>0.96546512071329205</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="23">
         <f>'Table 1 - copy raw data here'!I3</f>
         <v>0.87769876929967305</v>
       </c>
-      <c r="M4" s="16">
+      <c r="M4" s="24">
         <f>'Table 1 - copy raw data here'!J3</f>
         <v>0.63712450373597496</v>
       </c>
-      <c r="N4" s="42" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="20">
+      <c r="N4" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="65">
         <f>'Table 1 - copy raw data here'!E4</f>
         <v>1.5220841060619399</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="16">
         <f>'Table 1 - copy raw data here'!F4</f>
         <v>1.3702253440619401</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="17">
         <f>'Table 1 - copy raw data here'!G4</f>
         <v>1.2227832780619401</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="66">
         <f>'Table 1 - copy raw data here'!B4/100</f>
         <v>0.75</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="67">
         <f>'Table 1 - copy raw data here'!C4/100</f>
         <v>0.67500000000000004</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="68">
         <f>'Table 1 - copy raw data here'!D4/100</f>
         <v>0.60199999999999998</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="65">
         <f>'Table 1 - copy raw data here'!K4</f>
         <v>0.41951285242667402</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="16">
         <f>'Table 1 - copy raw data here'!L4</f>
         <v>0.46811426299519598</v>
       </c>
-      <c r="J5" s="21">
+      <c r="J5" s="16">
         <f>'Table 1 - copy raw data here'!M4</f>
         <v>0.33694581169332799</v>
       </c>
-      <c r="K5" s="36">
+      <c r="K5" s="69">
         <f>'Table 1 - copy raw data here'!H4</f>
         <v>0.98047507399070599</v>
       </c>
-      <c r="L5" s="94">
+      <c r="L5" s="70">
         <f>'Table 1 - copy raw data here'!I4</f>
         <v>0.93019406011203898</v>
       </c>
-      <c r="M5" s="22">
+      <c r="M5" s="17">
         <f>'Table 1 - copy raw data here'!J4</f>
         <v>0.67053346789159896</v>
       </c>
-      <c r="N5" s="41" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="88">
+      <c r="N5" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="71">
         <f>'Table 1 - copy raw data here'!E5</f>
         <v>0.83586382093317102</v>
       </c>
-      <c r="C6" s="89">
+      <c r="C6" s="72">
         <f>'Table 1 - copy raw data here'!F5</f>
         <v>0.60332796572881597</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="24">
         <f>'Table 1 - copy raw data here'!G5</f>
         <v>0.88872024081419099</v>
       </c>
-      <c r="E6" s="91">
+      <c r="E6" s="73">
         <f>'Table 1 - copy raw data here'!B5/100</f>
         <v>0.30099999999999999</v>
       </c>
-      <c r="F6" s="92">
+      <c r="F6" s="74">
         <f>'Table 1 - copy raw data here'!C5/100</f>
         <v>0.254</v>
       </c>
-      <c r="G6" s="93">
+      <c r="G6" s="75">
         <f>'Table 1 - copy raw data here'!D5/100</f>
         <v>0.188</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="61">
         <f>'Table 1 - copy raw data here'!K5</f>
         <v>0.35680908719869198</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="23">
         <f>'Table 1 - copy raw data here'!L5</f>
         <v>0.39691877484075699</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="23">
         <f>'Table 1 - copy raw data here'!M5</f>
         <v>0.30625140776853899</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="61">
         <f>'Table 1 - copy raw data here'!H5</f>
         <v>0.95987013370315999</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="23">
         <f>'Table 1 - copy raw data here'!I5</f>
         <v>0.88673729685160996</v>
       </c>
-      <c r="M6" s="95">
+      <c r="M6" s="76">
         <f>'Table 1 - copy raw data here'!J5</f>
         <v>0.71027998243946699</v>
       </c>
-      <c r="N6" s="40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="20">
+      <c r="N6" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="65">
         <f>'Table 1 - copy raw data here'!E6</f>
         <v>1.2791523360619399</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="16">
         <f>'Table 1 - copy raw data here'!F6</f>
         <v>1.11282718006194</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="17">
         <f>'Table 1 - copy raw data here'!G6</f>
         <v>1.0036873200619401</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="66">
         <f>'Table 1 - copy raw data here'!B6/100</f>
         <v>0.63</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="67">
         <f>'Table 1 - copy raw data here'!C6/100</f>
         <v>0.54799999999999993</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="68">
         <f>'Table 1 - copy raw data here'!D6/100</f>
         <v>0.49399999999999999</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="65">
         <f>'Table 1 - copy raw data here'!K6</f>
         <v>0.417700106510139</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="16">
         <f>'Table 1 - copy raw data here'!L6</f>
         <v>0.46456133905040398</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="16">
         <f>'Table 1 - copy raw data here'!M6</f>
         <v>0.32831283047439103</v>
       </c>
-      <c r="K7" s="36">
+      <c r="K7" s="69">
         <f>'Table 1 - copy raw data here'!H6</f>
         <v>0.97827409490972295</v>
       </c>
-      <c r="L7" s="21">
+      <c r="L7" s="16">
         <f>'Table 1 - copy raw data here'!I6</f>
         <v>0.91565097784484495</v>
       </c>
-      <c r="M7" s="22">
+      <c r="M7" s="17">
         <f>'Table 1 - copy raw data here'!J6</f>
         <v>0.64345323564458301</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="61">
         <f>'Table 1 - copy raw data here'!E7</f>
         <v>3.3609131600619402</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="23">
         <f>'Table 1 - copy raw data here'!F7</f>
         <v>2.9305214960619401</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="24">
         <f>'Table 1 - copy raw data here'!G7</f>
         <v>3.0432672320619401</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="62">
         <f>'Table 1 - copy raw data here'!B7/100</f>
         <v>1.6559999999999999</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="63">
         <f>'Table 1 - copy raw data here'!C7/100</f>
         <v>1.444</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="64">
         <f>'Table 1 - copy raw data here'!D7/100</f>
         <v>1.4990000000000001</v>
       </c>
-      <c r="H8" s="88">
+      <c r="H8" s="71">
         <f>'Table 1 - copy raw data here'!K7</f>
         <v>0.54931383902197095</v>
       </c>
-      <c r="I8" s="89">
+      <c r="I8" s="72">
         <f>'Table 1 - copy raw data here'!L7</f>
         <v>0.60926055216130204</v>
       </c>
-      <c r="J8" s="94">
+      <c r="J8" s="70">
         <f>'Table 1 - copy raw data here'!M7</f>
         <v>0.42013696880208601</v>
       </c>
-      <c r="K8" s="36">
+      <c r="K8" s="69">
         <f>'Table 1 - copy raw data here'!H7</f>
         <v>0.98400599280103296</v>
       </c>
-      <c r="L8" s="94">
+      <c r="L8" s="70">
         <f>'Table 1 - copy raw data here'!I7</f>
         <v>0.93078577029168597</v>
       </c>
-      <c r="M8" s="16">
+      <c r="M8" s="24">
         <f>'Table 1 - copy raw data here'!J7</f>
         <v>0.568102088811406</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="27">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="77">
         <f>'Table 1 - copy raw data here'!E8</f>
         <v>0.98815472206193999</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="37">
         <f>'Table 1 - copy raw data here'!F8</f>
         <v>1.2283358760619401</v>
       </c>
-      <c r="D9" s="90">
+      <c r="D9" s="78">
         <f>'Table 1 - copy raw data here'!G8</f>
         <v>0.86337590372881601</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="79">
         <f>'Table 1 - copy raw data here'!B8/100</f>
         <v>0.48700000000000004</v>
       </c>
-      <c r="F9" s="87">
+      <c r="F9" s="80">
         <f>'Table 1 - copy raw data here'!C8/100</f>
         <v>0.60499999999999998</v>
       </c>
-      <c r="G9" s="86">
+      <c r="G9" s="81">
         <f>'Table 1 - copy raw data here'!D8/100</f>
         <v>0.33899999999999997</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="77">
         <f>'Table 1 - copy raw data here'!K8</f>
         <v>0.441917209407449</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="37">
         <f>'Table 1 - copy raw data here'!L8</f>
         <v>0.48907248286788402</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="37">
         <f>'Table 1 - copy raw data here'!M8</f>
         <v>0.37111742539425402</v>
       </c>
-      <c r="K9" s="27">
+      <c r="K9" s="77">
         <f>'Table 1 - copy raw data here'!H8</f>
         <v>0.96972039389537301</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="37">
         <f>'Table 1 - copy raw data here'!I8</f>
         <v>0.90988591409012798</v>
       </c>
-      <c r="M9" s="85">
+      <c r="M9" s="38">
         <f>'Table 1 - copy raw data here'!J8</f>
         <v>0.69401816999657095</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="32">
+      <c r="A10" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="82">
         <f>AVERAGE(B3:B9)</f>
         <v>1.6453730527578301</v>
       </c>
-      <c r="C10" s="83">
+      <c r="C10" s="23">
         <f t="shared" ref="C10:M10" si="0">AVERAGE(C3:C9)</f>
         <v>1.4564653408714938</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="83">
         <f t="shared" si="0"/>
         <v>1.4390239191340108</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="84">
         <f t="shared" si="0"/>
         <v>0.79485714285714282</v>
       </c>
-      <c r="F10" s="84">
+      <c r="F10" s="85">
         <f t="shared" si="0"/>
         <v>0.71128571428571441</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="86">
         <f t="shared" si="0"/>
         <v>0.64900000000000013</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="82">
         <f t="shared" si="0"/>
         <v>0.42424791180768728</v>
       </c>
-      <c r="I10" s="37">
+      <c r="I10" s="83">
         <f t="shared" si="0"/>
         <v>0.46406106348177428</v>
       </c>
-      <c r="J10" s="83">
+      <c r="J10" s="23">
         <f t="shared" si="0"/>
         <v>0.32491716582232144</v>
       </c>
-      <c r="K10" s="39">
+      <c r="K10" s="87">
         <f t="shared" si="0"/>
         <v>0.93500486668490457</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="88">
         <f t="shared" si="0"/>
         <v>0.87739683236734556</v>
       </c>
-      <c r="M10" s="34">
+      <c r="M10" s="89">
         <f t="shared" si="0"/>
         <v>0.60587569612727754</v>
       </c>
@@ -1865,16 +1911,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2005,8 +2051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926FA25B-0675-4415-9EAE-A1DBC10ABC93}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2015,168 +2061,168 @@
     <col min="2" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="47">
+      <c r="A2" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="48">
         <f>'Table S1 copy raw data'!C2</f>
         <v>9.2940388488922707E-2</v>
       </c>
-      <c r="C2" s="48">
+      <c r="C2" s="49">
         <f>'Table S1 copy raw data'!B2</f>
         <v>0</v>
       </c>
-      <c r="D2" s="49">
+      <c r="D2" s="50">
         <f>'Table S1 copy raw data'!E2</f>
         <v>1.01020632147573</v>
       </c>
-      <c r="E2" s="50">
+      <c r="E2" s="51">
         <f>'Table S1 copy raw data'!D2</f>
         <v>0.95392405937265901</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="47">
+      <c r="A3" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="48">
         <f>'Table S1 copy raw data'!C3</f>
         <v>0.340981905337637</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="49">
         <f>'Table S1 copy raw data'!B3</f>
         <v>0</v>
       </c>
-      <c r="D3" s="49">
+      <c r="D3" s="50">
         <f>'Table S1 copy raw data'!E3</f>
         <v>0.564953094661791</v>
       </c>
-      <c r="E3" s="50">
+      <c r="E3" s="51">
         <f>'Table S1 copy raw data'!D3</f>
         <v>0.46154690097069101</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="47">
+      <c r="A4" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="48">
         <f>'Table S1 copy raw data'!C4</f>
         <v>0.16927279982131699</v>
       </c>
-      <c r="C4" s="48">
+      <c r="C4" s="49">
         <f>'Table S1 copy raw data'!B4</f>
         <v>0</v>
       </c>
-      <c r="D4" s="49">
+      <c r="D4" s="50">
         <f>'Table S1 copy raw data'!E4</f>
         <v>0.96916176826951494</v>
       </c>
-      <c r="E4" s="50">
+      <c r="E4" s="51">
         <f>'Table S1 copy raw data'!D4</f>
         <v>0.85119026125060704</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="47">
+      <c r="A5" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="48">
         <f>'Table S1 copy raw data'!C5</f>
         <v>0.18379400931050499</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="49">
         <f>'Table S1 copy raw data'!B5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="49">
+      <c r="D5" s="50">
         <f>'Table S1 copy raw data'!E5</f>
         <v>0.84537688322844495</v>
       </c>
-      <c r="E5" s="50">
+      <c r="E5" s="51">
         <f>'Table S1 copy raw data'!D5</f>
         <v>0.78498217394466796</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="47">
+      <c r="A6" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="48">
         <f>'Table S1 copy raw data'!C6</f>
         <v>0.122234561255987</v>
       </c>
-      <c r="C6" s="48">
+      <c r="C6" s="49">
         <f>'Table S1 copy raw data'!B6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="49">
+      <c r="D6" s="50">
         <f>'Table S1 copy raw data'!E6</f>
         <v>0.96072006766502605</v>
       </c>
-      <c r="E6" s="50">
+      <c r="E6" s="51">
         <f>'Table S1 copy raw data'!D6</f>
         <v>0.90151033916294798</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="47">
+      <c r="A7" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="48">
         <f>'Table S1 copy raw data'!C7</f>
         <v>0.10041277669412101</v>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="49">
         <f>'Table S1 copy raw data'!B7</f>
         <v>0</v>
       </c>
-      <c r="D7" s="49">
+      <c r="D7" s="50">
         <f>'Table S1 copy raw data'!E7</f>
         <v>1.0199820836896401</v>
       </c>
-      <c r="E7" s="50">
+      <c r="E7" s="51">
         <f>'Table S1 copy raw data'!D7</f>
         <v>0.94946093017919098</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="47">
+      <c r="A8" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="48">
         <f>'Table S1 copy raw data'!C8</f>
         <v>0.13208980592191499</v>
       </c>
-      <c r="C8" s="48">
+      <c r="C8" s="49">
         <f>'Table S1 copy raw data'!B8</f>
         <v>0</v>
       </c>
-      <c r="D8" s="49">
+      <c r="D8" s="50">
         <f>'Table S1 copy raw data'!E8</f>
         <v>0.96124285380409002</v>
       </c>
-      <c r="E8" s="50">
+      <c r="E8" s="51">
         <f>'Table S1 copy raw data'!D8</f>
         <v>0.89369366323562704</v>
       </c>
@@ -2201,19 +2247,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2373,7 +2419,7 @@
         <v>0.87094991566539404</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2393,7 +2439,7 @@
         <v>0.72327523984244202</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2413,7 +2459,7 @@
         <v>0.94534026810471095</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2433,7 +2479,7 @@
         <v>0.89084759779255096</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2453,7 +2499,7 @@
         <v>0.649411350496922</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2473,7 +2519,7 @@
         <v>0.51385254197861896</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2493,7 +2539,7 @@
         <v>1.0560030090570101</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2505,365 +2551,1042 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC122BAA-6B80-44F9-A1DF-409EA6AE6532}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="51"/>
-      <c r="B1" s="81" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="81" t="s">
+    <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="93"/>
+      <c r="B1" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="92"/>
+      <c r="D1" s="91" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="92"/>
+      <c r="F1" s="91" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="92"/>
+      <c r="H1" s="91" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="92"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="82"/>
-      <c r="F1" s="81" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="82"/>
-      <c r="H1" s="81" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="82"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="55" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="68">
+      <c r="B3" s="12">
         <f>'Table 2 - copy raw data here'!C2</f>
         <v>145.63510790120901</v>
       </c>
-      <c r="C3" s="69">
+      <c r="C3" s="13">
         <f>'Table 2 - copy raw data here'!C9</f>
         <v>98.874492262887699</v>
       </c>
-      <c r="D3" s="70">
+      <c r="D3" s="14">
         <f>'Table 2 - copy raw data here'!B2</f>
         <v>14.7</v>
       </c>
-      <c r="E3" s="71">
+      <c r="E3" s="15">
         <f>'Table 2 - copy raw data here'!B9</f>
         <v>12.2</v>
       </c>
-      <c r="F3" s="72">
+      <c r="F3" s="16">
         <f>'Table 2 - copy raw data here'!E2</f>
         <v>0.47014517086380903</v>
       </c>
-      <c r="G3" s="73">
+      <c r="G3" s="17">
         <f>'Table 2 - copy raw data here'!E9</f>
         <v>0.87094991566539404</v>
       </c>
-      <c r="H3" s="72">
+      <c r="H3" s="16">
         <f>'Table 2 - copy raw data here'!D2</f>
         <v>0.16558424807591199</v>
       </c>
-      <c r="I3" s="73">
+      <c r="I3" s="17">
         <f>'Table 2 - copy raw data here'!D9</f>
         <v>0.35674008376359601</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="56">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="19">
         <f>'Table 2 - copy raw data here'!C3</f>
         <v>222.54464309897301</v>
       </c>
-      <c r="C4" s="57">
+      <c r="C4" s="20">
         <f>'Table 2 - copy raw data here'!C10</f>
         <v>190.131853581462</v>
       </c>
-      <c r="D4" s="58">
+      <c r="D4" s="21">
         <f>'Table 2 - copy raw data here'!B3</f>
         <v>53</v>
       </c>
-      <c r="E4" s="59">
+      <c r="E4" s="22">
         <f>'Table 2 - copy raw data here'!B10</f>
         <v>49.6</v>
       </c>
-      <c r="F4" s="60">
+      <c r="F4" s="23">
         <f>'Table 2 - copy raw data here'!E3</f>
         <v>0.32618257824870001</v>
       </c>
-      <c r="G4" s="61">
+      <c r="G4" s="24">
         <f>'Table 2 - copy raw data here'!E10</f>
         <v>0.72327523984244202</v>
       </c>
-      <c r="H4" s="60">
+      <c r="H4" s="23">
         <f>'Table 2 - copy raw data here'!D3</f>
         <v>0.159415768085021</v>
       </c>
-      <c r="I4" s="61">
+      <c r="I4" s="24">
         <f>'Table 2 - copy raw data here'!D10</f>
         <v>0.424228374684327</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="68">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="12">
         <f>'Table 2 - copy raw data here'!C4</f>
         <v>142.75054632827599</v>
       </c>
-      <c r="C5" s="69">
+      <c r="C5" s="13">
         <f>'Table 2 - copy raw data here'!C11</f>
         <v>99.603747299688393</v>
       </c>
-      <c r="D5" s="70">
+      <c r="D5" s="14">
         <f>'Table 2 - copy raw data here'!B4</f>
         <v>16.899999999999999</v>
       </c>
-      <c r="E5" s="71">
+      <c r="E5" s="15">
         <f>'Table 2 - copy raw data here'!B11</f>
         <v>14.4</v>
       </c>
-      <c r="F5" s="72">
+      <c r="F5" s="16">
         <f>'Table 2 - copy raw data here'!E4</f>
         <v>0.52362784643197202</v>
       </c>
-      <c r="G5" s="73">
+      <c r="G5" s="17">
         <f>'Table 2 - copy raw data here'!E11</f>
         <v>0.94534026810471095</v>
       </c>
-      <c r="H5" s="72">
+      <c r="H5" s="16">
         <f>'Table 2 - copy raw data here'!D4</f>
         <v>0.199570171231125</v>
       </c>
-      <c r="I5" s="73">
+      <c r="I5" s="17">
         <f>'Table 2 - copy raw data here'!D11</f>
         <v>0.39908717943623601</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="56">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="19">
         <f>'Table 2 - copy raw data here'!C5</f>
         <v>157.47284111953701</v>
       </c>
-      <c r="C6" s="57">
+      <c r="C6" s="20">
         <f>'Table 2 - copy raw data here'!C12</f>
         <v>123.92817748618199</v>
       </c>
-      <c r="D6" s="58">
+      <c r="D6" s="21">
         <f>'Table 2 - copy raw data here'!B5</f>
         <v>-29.5</v>
       </c>
-      <c r="E6" s="59">
+      <c r="E6" s="22">
         <f>'Table 2 - copy raw data here'!B12</f>
         <v>-31.3</v>
       </c>
-      <c r="F6" s="60">
+      <c r="F6" s="23">
         <f>'Table 2 - copy raw data here'!E5</f>
         <v>0.54043995425047398</v>
       </c>
-      <c r="G6" s="61">
+      <c r="G6" s="24">
         <f>'Table 2 - copy raw data here'!E12</f>
         <v>0.89084759779255096</v>
       </c>
-      <c r="H6" s="60">
+      <c r="H6" s="23">
         <f>'Table 2 - copy raw data here'!D5</f>
         <v>0.21098245367756199</v>
       </c>
-      <c r="I6" s="61">
+      <c r="I6" s="24">
         <f>'Table 2 - copy raw data here'!D12</f>
         <v>0.373040091440559</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="68">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="12">
         <f>'Table 2 - copy raw data here'!C6</f>
         <v>139.66097462927701</v>
       </c>
-      <c r="C7" s="69">
+      <c r="C7" s="13">
         <f>'Table 2 - copy raw data here'!C13</f>
         <v>101.649558801711</v>
       </c>
-      <c r="D7" s="70">
+      <c r="D7" s="14">
         <f>'Table 2 - copy raw data here'!B6</f>
         <v>-0.9</v>
       </c>
-      <c r="E7" s="71">
+      <c r="E7" s="15">
         <f>'Table 2 - copy raw data here'!B13</f>
         <v>-3.3</v>
       </c>
-      <c r="F7" s="72">
+      <c r="F7" s="16">
         <f>'Table 2 - copy raw data here'!E6</f>
         <v>0.46981089329105102</v>
       </c>
-      <c r="G7" s="73">
+      <c r="G7" s="17">
         <f>'Table 2 - copy raw data here'!E13</f>
         <v>0.649411350496922</v>
       </c>
-      <c r="H7" s="72">
+      <c r="H7" s="16">
         <f>'Table 2 - copy raw data here'!D6</f>
         <v>0.113886370151475</v>
       </c>
-      <c r="I7" s="73">
+      <c r="I7" s="17">
         <f>'Table 2 - copy raw data here'!D13</f>
         <v>0.169274581569167</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="56">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="19">
         <f>'Table 2 - copy raw data here'!C7</f>
         <v>279.56460329244601</v>
       </c>
-      <c r="C8" s="57">
+      <c r="C8" s="20">
         <f>'Table 2 - copy raw data here'!C14</f>
         <v>258.99252047032201</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="21">
         <f>'Table 2 - copy raw data here'!B7</f>
         <v>72.400000000000006</v>
       </c>
-      <c r="E8" s="59">
+      <c r="E8" s="22">
         <f>'Table 2 - copy raw data here'!B14</f>
         <v>68.2</v>
       </c>
-      <c r="F8" s="60">
+      <c r="F8" s="23">
         <f>'Table 2 - copy raw data here'!E7</f>
         <v>0.27856920003521501</v>
       </c>
-      <c r="G8" s="61">
+      <c r="G8" s="24">
         <f>'Table 2 - copy raw data here'!E14</f>
         <v>0.51385254197861896</v>
       </c>
-      <c r="H8" s="60">
+      <c r="H8" s="23">
         <f>'Table 2 - copy raw data here'!D7</f>
         <v>6.15220402826121E-2</v>
       </c>
-      <c r="I8" s="61">
+      <c r="I8" s="24">
         <f>'Table 2 - copy raw data here'!D14</f>
         <v>0.12538173855728399</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="74">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="33">
         <f>'Table 2 - copy raw data here'!C8</f>
         <v>144.341525553043</v>
       </c>
-      <c r="C9" s="75">
+      <c r="C9" s="34">
         <f>'Table 2 - copy raw data here'!C15</f>
         <v>89.848002117268393</v>
       </c>
-      <c r="D9" s="76">
+      <c r="D9" s="35">
         <f>'Table 2 - copy raw data here'!B8</f>
         <v>16.7</v>
       </c>
-      <c r="E9" s="77">
+      <c r="E9" s="36">
         <f>'Table 2 - copy raw data here'!B15</f>
         <v>14.4</v>
       </c>
-      <c r="F9" s="78">
+      <c r="F9" s="37">
         <f>'Table 2 - copy raw data here'!E8</f>
         <v>0.48963860411815502</v>
       </c>
-      <c r="G9" s="79">
+      <c r="G9" s="38">
         <f>'Table 2 - copy raw data here'!E15</f>
         <v>1.0560030090570101</v>
       </c>
-      <c r="H9" s="78">
+      <c r="H9" s="37">
         <f>'Table 2 - copy raw data here'!D8</f>
         <v>0.24086493137075801</v>
       </c>
-      <c r="I9" s="79">
+      <c r="I9" s="38">
         <f>'Table 2 - copy raw data here'!D15</f>
         <v>0.56024285483421699</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="62">
+      <c r="A10" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="39">
         <f>AVERAGE(B3:B9)</f>
         <v>175.99574884610871</v>
       </c>
-      <c r="C10" s="63">
+      <c r="C10" s="40">
         <f t="shared" ref="C10:I10" si="0">AVERAGE(C3:C9)</f>
         <v>137.57547885993162</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="41">
         <f t="shared" si="0"/>
         <v>20.471428571428568</v>
       </c>
-      <c r="E10" s="65">
+      <c r="E10" s="42">
         <f t="shared" si="0"/>
         <v>17.742857142857144</v>
       </c>
-      <c r="F10" s="66">
+      <c r="F10" s="43">
         <f t="shared" si="0"/>
         <v>0.44263060674848231</v>
       </c>
-      <c r="G10" s="67">
+      <c r="G10" s="44">
         <f t="shared" si="0"/>
         <v>0.80709713184823573</v>
       </c>
-      <c r="H10" s="66">
+      <c r="H10" s="43">
         <f t="shared" si="0"/>
         <v>0.16454656898206643</v>
       </c>
-      <c r="I10" s="67">
+      <c r="I10" s="44">
         <f t="shared" si="0"/>
         <v>0.34399927204076947</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3187032F-1B6C-4E62-935E-29A85F8C99C3}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>-2.1</v>
+      </c>
+      <c r="C2">
+        <v>158.83670079153501</v>
+      </c>
+      <c r="D2">
+        <v>0.14925647947771201</v>
+      </c>
+      <c r="E2">
+        <v>0.36435489412809002</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="C3">
+        <v>208.573091116265</v>
+      </c>
+      <c r="D3">
+        <v>0.15191706857592699</v>
+      </c>
+      <c r="E3">
+        <v>0.27763651089607999</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="C4">
+        <v>154.24716734549</v>
+      </c>
+      <c r="D4">
+        <v>0.17553976672256899</v>
+      </c>
+      <c r="E4">
+        <v>0.39957897070387199</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>-44.3</v>
+      </c>
+      <c r="C5">
+        <v>193.51904132870399</v>
+      </c>
+      <c r="D5">
+        <v>0.20022441309066299</v>
+      </c>
+      <c r="E5">
+        <v>0.46786228323747497</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>-17.600000000000001</v>
+      </c>
+      <c r="C6">
+        <v>160.428672913577</v>
+      </c>
+      <c r="D6">
+        <v>0.110529415139272</v>
+      </c>
+      <c r="E6">
+        <v>0.36863747561622201</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>55.5</v>
+      </c>
+      <c r="C7">
+        <v>237.034461967254</v>
+      </c>
+      <c r="D7">
+        <v>6.5466048596065501E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.234391905366129</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>0.2</v>
+      </c>
+      <c r="C8">
+        <v>157.78847803505801</v>
+      </c>
+      <c r="D8">
+        <v>0.21200295801792801</v>
+      </c>
+      <c r="E8">
+        <v>0.39201007916068698</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>-3.7</v>
+      </c>
+      <c r="C9">
+        <v>86.676236646068105</v>
+      </c>
+      <c r="D9">
+        <v>0.40106600584448998</v>
+      </c>
+      <c r="E9">
+        <v>0.86164404835919906</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>33.6</v>
+      </c>
+      <c r="C10">
+        <v>140.09986888491301</v>
+      </c>
+      <c r="D10">
+        <v>0.44557669366817398</v>
+      </c>
+      <c r="E10">
+        <v>0.69282968059709704</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>-1.5</v>
+      </c>
+      <c r="C11">
+        <v>84.810872632814394</v>
+      </c>
+      <c r="D11">
+        <v>0.43513330302387698</v>
+      </c>
+      <c r="E11">
+        <v>0.90921286467112905</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>-45.3</v>
+      </c>
+      <c r="C12">
+        <v>168.690255571888</v>
+      </c>
+      <c r="D12">
+        <v>0.44003666382415402</v>
+      </c>
+      <c r="E12">
+        <v>0.97362933474074598</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>-19.2</v>
+      </c>
+      <c r="C13">
+        <v>99.039687311519501</v>
+      </c>
+      <c r="D13">
+        <v>0.214710871542101</v>
+      </c>
+      <c r="E13">
+        <v>0.67864264295438703</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>52.2</v>
+      </c>
+      <c r="C14">
+        <v>204.40437071949901</v>
+      </c>
+      <c r="D14">
+        <v>0.16307516295921401</v>
+      </c>
+      <c r="E14">
+        <v>0.54285206096132699</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>-1.3</v>
+      </c>
+      <c r="C15">
+        <v>61.825709179357297</v>
+      </c>
+      <c r="D15">
+        <v>0.60633357551690403</v>
+      </c>
+      <c r="E15">
+        <v>1.0380621339618601</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36A2F12F-391E-4BF3-B795-06EB170EE646}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="A1:I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="92"/>
+      <c r="D1" s="91" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="92"/>
+      <c r="F1" s="91" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="92"/>
+      <c r="H1" s="91" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="92"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="12">
+        <f>'Table S2 - copy raw data here'!C2</f>
+        <v>158.83670079153501</v>
+      </c>
+      <c r="C3" s="13">
+        <f>'Table S2 - copy raw data here'!C9</f>
+        <v>86.676236646068105</v>
+      </c>
+      <c r="D3" s="14">
+        <f>'Table S2 - copy raw data here'!B2</f>
+        <v>-2.1</v>
+      </c>
+      <c r="E3" s="15">
+        <f>'Table S2 - copy raw data here'!B9</f>
+        <v>-3.7</v>
+      </c>
+      <c r="F3" s="16">
+        <f>'Table S2 - copy raw data here'!E2</f>
+        <v>0.36435489412809002</v>
+      </c>
+      <c r="G3" s="17">
+        <f>'Table S2 - copy raw data here'!E9</f>
+        <v>0.86164404835919906</v>
+      </c>
+      <c r="H3" s="16">
+        <f>'Table S2 - copy raw data here'!D2</f>
+        <v>0.14925647947771201</v>
+      </c>
+      <c r="I3" s="17">
+        <f>'Table S2 - copy raw data here'!D9</f>
+        <v>0.40106600584448998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="19">
+        <f>'Table S2 - copy raw data here'!C3</f>
+        <v>208.573091116265</v>
+      </c>
+      <c r="C4" s="20">
+        <f>'Table S2 - copy raw data here'!C10</f>
+        <v>140.09986888491301</v>
+      </c>
+      <c r="D4" s="21">
+        <f>'Table S2 - copy raw data here'!B3</f>
+        <v>36.200000000000003</v>
+      </c>
+      <c r="E4" s="22">
+        <f>'Table S2 - copy raw data here'!B10</f>
+        <v>33.6</v>
+      </c>
+      <c r="F4" s="23">
+        <f>'Table S2 - copy raw data here'!E3</f>
+        <v>0.27763651089607999</v>
+      </c>
+      <c r="G4" s="24">
+        <f>'Table S2 - copy raw data here'!E10</f>
+        <v>0.69282968059709704</v>
+      </c>
+      <c r="H4" s="23">
+        <f>'Table S2 - copy raw data here'!D3</f>
+        <v>0.15191706857592699</v>
+      </c>
+      <c r="I4" s="24">
+        <f>'Table S2 - copy raw data here'!D10</f>
+        <v>0.44557669366817398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="12">
+        <f>'Table S2 - copy raw data here'!C4</f>
+        <v>154.24716734549</v>
+      </c>
+      <c r="C5" s="13">
+        <f>'Table S2 - copy raw data here'!C11</f>
+        <v>84.810872632814394</v>
+      </c>
+      <c r="D5" s="14">
+        <f>'Table S2 - copy raw data here'!B4</f>
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="15">
+        <f>'Table S2 - copy raw data here'!B11</f>
+        <v>-1.5</v>
+      </c>
+      <c r="F5" s="16">
+        <f>'Table S2 - copy raw data here'!E4</f>
+        <v>0.39957897070387199</v>
+      </c>
+      <c r="G5" s="17">
+        <f>'Table S2 - copy raw data here'!E11</f>
+        <v>0.90921286467112905</v>
+      </c>
+      <c r="H5" s="16">
+        <f>'Table S2 - copy raw data here'!D4</f>
+        <v>0.17553976672256899</v>
+      </c>
+      <c r="I5" s="17">
+        <f>'Table S2 - copy raw data here'!D11</f>
+        <v>0.43513330302387698</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="19">
+        <f>'Table S2 - copy raw data here'!C5</f>
+        <v>193.51904132870399</v>
+      </c>
+      <c r="C6" s="20">
+        <f>'Table S2 - copy raw data here'!C12</f>
+        <v>168.690255571888</v>
+      </c>
+      <c r="D6" s="21">
+        <f>'Table S2 - copy raw data here'!B5</f>
+        <v>-44.3</v>
+      </c>
+      <c r="E6" s="22">
+        <f>'Table S2 - copy raw data here'!B12</f>
+        <v>-45.3</v>
+      </c>
+      <c r="F6" s="23">
+        <f>'Table S2 - copy raw data here'!E5</f>
+        <v>0.46786228323747497</v>
+      </c>
+      <c r="G6" s="24">
+        <f>'Table S2 - copy raw data here'!E12</f>
+        <v>0.97362933474074598</v>
+      </c>
+      <c r="H6" s="23">
+        <f>'Table S2 - copy raw data here'!D5</f>
+        <v>0.20022441309066299</v>
+      </c>
+      <c r="I6" s="24">
+        <f>'Table S2 - copy raw data here'!D12</f>
+        <v>0.44003666382415402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="12">
+        <f>'Table S2 - copy raw data here'!C6</f>
+        <v>160.428672913577</v>
+      </c>
+      <c r="C7" s="13">
+        <f>'Table S2 - copy raw data here'!C13</f>
+        <v>99.039687311519501</v>
+      </c>
+      <c r="D7" s="14">
+        <f>'Table S2 - copy raw data here'!B6</f>
+        <v>-17.600000000000001</v>
+      </c>
+      <c r="E7" s="15">
+        <f>'Table S2 - copy raw data here'!B13</f>
+        <v>-19.2</v>
+      </c>
+      <c r="F7" s="16">
+        <f>'Table S2 - copy raw data here'!E6</f>
+        <v>0.36863747561622201</v>
+      </c>
+      <c r="G7" s="17">
+        <f>'Table S2 - copy raw data here'!E13</f>
+        <v>0.67864264295438703</v>
+      </c>
+      <c r="H7" s="16">
+        <f>'Table S2 - copy raw data here'!D6</f>
+        <v>0.110529415139272</v>
+      </c>
+      <c r="I7" s="17">
+        <f>'Table S2 - copy raw data here'!D13</f>
+        <v>0.214710871542101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="19">
+        <f>'Table S2 - copy raw data here'!C7</f>
+        <v>237.034461967254</v>
+      </c>
+      <c r="C8" s="20">
+        <f>'Table S2 - copy raw data here'!C14</f>
+        <v>204.40437071949901</v>
+      </c>
+      <c r="D8" s="21">
+        <f>'Table S2 - copy raw data here'!B7</f>
+        <v>55.5</v>
+      </c>
+      <c r="E8" s="22">
+        <f>'Table S2 - copy raw data here'!B14</f>
+        <v>52.2</v>
+      </c>
+      <c r="F8" s="23">
+        <f>'Table S2 - copy raw data here'!E7</f>
+        <v>0.234391905366129</v>
+      </c>
+      <c r="G8" s="24">
+        <f>'Table S2 - copy raw data here'!E14</f>
+        <v>0.54285206096132699</v>
+      </c>
+      <c r="H8" s="23">
+        <f>'Table S2 - copy raw data here'!D7</f>
+        <v>6.5466048596065501E-2</v>
+      </c>
+      <c r="I8" s="24">
+        <f>'Table S2 - copy raw data here'!D14</f>
+        <v>0.16307516295921401</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="12">
+        <f>'Table S2 - copy raw data here'!C8</f>
+        <v>157.78847803505801</v>
+      </c>
+      <c r="C9" s="13">
+        <f>'Table S2 - copy raw data here'!C15</f>
+        <v>61.825709179357297</v>
+      </c>
+      <c r="D9" s="14">
+        <f>'Table S2 - copy raw data here'!B8</f>
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="15">
+        <f>'Table S2 - copy raw data here'!B15</f>
+        <v>-1.3</v>
+      </c>
+      <c r="F9" s="16">
+        <f>'Table S2 - copy raw data here'!E8</f>
+        <v>0.39201007916068698</v>
+      </c>
+      <c r="G9" s="17">
+        <f>'Table S2 - copy raw data here'!E15</f>
+        <v>1.0380621339618601</v>
+      </c>
+      <c r="H9" s="16">
+        <f>'Table S2 - copy raw data here'!D8</f>
+        <v>0.21200295801792801</v>
+      </c>
+      <c r="I9" s="17">
+        <f>'Table S2 - copy raw data here'!D15</f>
+        <v>0.60633357551690403</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="27">
+        <f>AVERAGE(B3:B9)</f>
+        <v>181.48965907112614</v>
+      </c>
+      <c r="C10" s="28">
+        <f t="shared" ref="C10:I10" si="0">AVERAGE(C3:C9)</f>
+        <v>120.79242870657991</v>
+      </c>
+      <c r="D10" s="29">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000009</v>
+      </c>
+      <c r="E10" s="30">
+        <f t="shared" si="0"/>
+        <v>2.1142857142857152</v>
+      </c>
+      <c r="F10" s="31">
+        <f t="shared" si="0"/>
+        <v>0.35778173130122209</v>
+      </c>
+      <c r="G10" s="32">
+        <f t="shared" si="0"/>
+        <v>0.81383896660653499</v>
+      </c>
+      <c r="H10" s="31">
+        <f t="shared" si="0"/>
+        <v>0.1521337356600195</v>
+      </c>
+      <c r="I10" s="32">
+        <f t="shared" si="0"/>
+        <v>0.38656175376841634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>